<commit_message>
Updated some measurements and resolved file path issues
</commit_message>
<xml_diff>
--- a/kalmax/data/games.xlsx
+++ b/kalmax/data/games.xlsx
@@ -272,6 +272,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <sz val="10.0"/>
@@ -299,14 +302,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -534,10 +540,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -545,10 +551,10 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>4.0</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="3">
         <f>9+7/8</f>
         <v>9.875</v>
       </c>
@@ -557,10 +563,10 @@
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3" s="2">
         <v>5.0</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="3">
         <f>1 + 3/8</f>
         <v>1.375</v>
       </c>
@@ -569,10 +575,10 @@
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4" s="2">
         <v>12.25</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>6.25</v>
       </c>
     </row>
@@ -580,11 +586,11 @@
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="3">
         <f> 5 + 13/16</f>
         <v>5.8125</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="3">
         <f>1 + 13/16</f>
         <v>1.8125</v>
       </c>
@@ -593,10 +599,10 @@
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6" s="2">
         <v>12.25</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="3">
         <f>3 + 1/8</f>
         <v>3.125</v>
       </c>
@@ -605,11 +611,11 @@
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="3">
         <f>9+1/16</f>
         <v>9.0625</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <f>1 + 13/16</f>
         <v>1.8125</v>
       </c>
@@ -618,10 +624,10 @@
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8" s="2">
         <v>6.0</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <f>1+5/8</f>
         <v>1.625</v>
       </c>
@@ -630,11 +636,11 @@
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="3">
         <f>4+3/16</f>
         <v>4.1875</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <f>1+9/16</f>
         <v>1.5625</v>
       </c>
@@ -643,10 +649,10 @@
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10" s="2">
         <v>11.75</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <f>2+7/8</f>
         <v>2.875</v>
       </c>
@@ -655,10 +661,10 @@
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11" s="2">
         <v>11.75</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <f>4+1/16</f>
         <v>4.0625</v>
       </c>
@@ -667,10 +673,10 @@
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12" s="2">
         <v>11.75</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <f>2+13/16</f>
         <v>2.8125</v>
       </c>
@@ -679,11 +685,11 @@
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="3">
         <f>11+11/16</f>
         <v>11.6875</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>3.25</v>
       </c>
     </row>
@@ -691,11 +697,11 @@
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14" s="2">
         <f>5+1/8</f>
         <v>5.125</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>1.5</v>
       </c>
     </row>
@@ -703,11 +709,11 @@
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="3">
         <f>5+5/8</f>
         <v>5.625</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>1.75</v>
       </c>
     </row>
@@ -715,11 +721,11 @@
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="3">
         <f>4+3/8</f>
         <v>4.375</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>4.5</v>
       </c>
     </row>
@@ -727,11 +733,11 @@
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="3">
         <f>1+9/16</f>
         <v>1.5625</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <f>9+7/16</f>
         <v>9.4375</v>
       </c>
@@ -740,10 +746,10 @@
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18" s="2">
         <v>6.25</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>2.125</v>
       </c>
     </row>
@@ -751,10 +757,10 @@
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19" s="2">
         <v>6.0</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <f>2+1/16</f>
         <v>2.0625</v>
       </c>
@@ -763,10 +769,10 @@
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="2">
         <v>10.0</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -774,10 +780,10 @@
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="2">
         <v>10.5</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -785,22 +791,22 @@
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="3">
         <f>8+3/16</f>
         <v>8.1875</v>
       </c>
-      <c r="C22" s="1">
-        <v>1.75</v>
+      <c r="C22" s="2">
+        <v>1.8125</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="2">
         <v>8.75</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <f>1 + 13/16</f>
         <v>1.8125</v>
       </c>
@@ -809,11 +815,11 @@
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="3">
         <f>8+7/8</f>
         <v>8.875</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>2.75</v>
       </c>
     </row>
@@ -821,10 +827,10 @@
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25" s="2">
         <v>9.0</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>4.0</v>
       </c>
     </row>
@@ -832,10 +838,10 @@
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26" s="2">
         <v>5.25</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>1.5</v>
       </c>
     </row>
@@ -843,10 +849,10 @@
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27" s="2">
         <v>10.5</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <f>2+5/8</f>
         <v>2.625</v>
       </c>
@@ -855,10 +861,10 @@
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28" s="2">
         <v>10.5</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>2.75</v>
       </c>
     </row>
@@ -866,10 +872,10 @@
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29" s="2">
         <v>7.0</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <f>1+5/8</f>
         <v>1.625</v>
       </c>
@@ -878,11 +884,11 @@
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="3">
         <f>11+5/8</f>
         <v>11.625</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <f>2+7/8</f>
         <v>2.875</v>
       </c>
@@ -891,10 +897,10 @@
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31" s="2">
         <v>3.0</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <v>10.75</v>
       </c>
     </row>
@@ -902,10 +908,10 @@
       <c r="A32" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32" s="2">
         <v>11.125</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <f>4+3/16</f>
         <v>4.1875</v>
       </c>
@@ -914,10 +920,10 @@
       <c r="A33" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33" s="2">
         <v>11.0</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33" s="2">
         <v>2.5</v>
       </c>
     </row>
@@ -925,11 +931,11 @@
       <c r="A34" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B34" s="2">
+      <c r="B34" s="3">
         <f>6+13/16</f>
         <v>6.8125</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <f>2+1/16</f>
         <v>2.0625</v>
       </c>
@@ -938,10 +944,10 @@
       <c r="A35" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35" s="2">
         <v>5.0</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35" s="2">
         <v>1.5</v>
       </c>
     </row>
@@ -949,11 +955,11 @@
       <c r="A36" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="2">
+      <c r="B36" s="3">
         <f>7+7/16</f>
         <v>7.4375</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36" s="2">
         <v>2.5</v>
       </c>
     </row>
@@ -961,10 +967,10 @@
       <c r="A37" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37" s="2">
         <v>8.0</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37" s="2">
         <v>2.5</v>
       </c>
     </row>
@@ -972,10 +978,10 @@
       <c r="A38" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38" s="2">
         <v>9.25</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <f t="shared" ref="C38:C39" si="1">2+7/8</f>
         <v>2.875</v>
       </c>
@@ -984,10 +990,10 @@
       <c r="A39" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39" s="2">
         <v>11.75</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <f t="shared" si="1"/>
         <v>2.875</v>
       </c>
@@ -996,11 +1002,11 @@
       <c r="A40" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B40" s="2">
+      <c r="B40" s="3">
         <f>11+7/8</f>
         <v>11.875</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -1008,10 +1014,10 @@
       <c r="A41" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41" s="2">
         <v>9.25</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="3">
         <f>2+13/16</f>
         <v>2.8125</v>
       </c>
@@ -1020,10 +1026,10 @@
       <c r="A42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42" s="2">
         <v>10.0</v>
       </c>
-      <c r="C42" s="1">
+      <c r="C42" s="2">
         <v>3.125</v>
       </c>
     </row>
@@ -1031,10 +1037,10 @@
       <c r="A43" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43" s="2">
         <v>11.75</v>
       </c>
-      <c r="C43" s="2">
+      <c r="C43" s="3">
         <f>3+5/16</f>
         <v>3.3125</v>
       </c>
@@ -1043,10 +1049,10 @@
       <c r="A44" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44" s="2">
         <v>10.0</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -1054,11 +1060,11 @@
       <c r="A45" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B45" s="2">
+      <c r="B45" s="3">
         <f>5+5/16</f>
         <v>5.3125</v>
       </c>
-      <c r="C45" s="2">
+      <c r="C45" s="3">
         <f>1 + 13/16</f>
         <v>1.8125</v>
       </c>
@@ -1067,10 +1073,10 @@
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46" s="2">
         <v>10.5</v>
       </c>
-      <c r="C46" s="2">
+      <c r="C46" s="3">
         <f>2+5/8</f>
         <v>2.625</v>
       </c>
@@ -1079,11 +1085,11 @@
       <c r="A47" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B47" s="2">
+      <c r="B47" s="3">
         <f>3+15/16</f>
         <v>3.9375</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47" s="2">
         <v>1.125</v>
       </c>
     </row>
@@ -1091,11 +1097,11 @@
       <c r="A48" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="3">
         <f>1+9/16</f>
         <v>1.5625</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48" s="2">
         <v>7.125</v>
       </c>
     </row>
@@ -1103,10 +1109,10 @@
       <c r="A49" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49" s="2">
         <v>7.5</v>
       </c>
-      <c r="C49" s="2">
+      <c r="C49" s="3">
         <f>2+5/8</f>
         <v>2.625</v>
       </c>
@@ -1115,11 +1121,11 @@
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B50" s="2">
+      <c r="B50" s="3">
         <f>11+7/8</f>
         <v>11.875</v>
       </c>
-      <c r="C50" s="2">
+      <c r="C50" s="3">
         <f>2.875</f>
         <v>2.875</v>
       </c>
@@ -1128,10 +1134,10 @@
       <c r="A51" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51" s="2">
         <v>10.5</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -1139,11 +1145,11 @@
       <c r="A52" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B52" s="2">
+      <c r="B52" s="3">
         <f t="shared" ref="B52:B53" si="2">10+7/8</f>
         <v>10.875</v>
       </c>
-      <c r="C52" s="2">
+      <c r="C52" s="3">
         <f t="shared" ref="C52:C53" si="3">2+3/16</f>
         <v>2.1875</v>
       </c>
@@ -1152,11 +1158,11 @@
       <c r="A53" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B53" s="2">
+      <c r="B53" s="3">
         <f t="shared" si="2"/>
         <v>10.875</v>
       </c>
-      <c r="C53" s="2">
+      <c r="C53" s="3">
         <f t="shared" si="3"/>
         <v>2.1875</v>
       </c>
@@ -1165,10 +1171,10 @@
       <c r="A54" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54" s="2">
         <v>8.125</v>
       </c>
-      <c r="C54" s="2">
+      <c r="C54" s="3">
         <f>1+7/8</f>
         <v>1.875</v>
       </c>
@@ -1177,10 +1183,10 @@
       <c r="A55" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55" s="2">
         <v>12.25</v>
       </c>
-      <c r="C55" s="2">
+      <c r="C55" s="3">
         <f>2+3/16</f>
         <v>2.1875</v>
       </c>
@@ -1189,11 +1195,11 @@
       <c r="A56" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56" s="2">
         <f t="shared" ref="B56:B57" si="4">11+5/8</f>
         <v>11.625</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56" s="2">
         <v>2.75</v>
       </c>
     </row>
@@ -1201,11 +1207,11 @@
       <c r="A57" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="2">
+      <c r="B57" s="3">
         <f t="shared" si="4"/>
         <v>11.625</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -1213,11 +1219,11 @@
       <c r="A58" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B58" s="3">
         <f>12+13/16</f>
         <v>12.8125</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58" s="2">
         <v>3.5</v>
       </c>
     </row>
@@ -1225,11 +1231,11 @@
       <c r="A59" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B59" s="2">
+      <c r="B59" s="3">
         <f>2+7/8</f>
         <v>2.875</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59" s="2">
         <v>8.25</v>
       </c>
     </row>
@@ -1237,10 +1243,10 @@
       <c r="A60" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60" s="2">
         <v>8.5</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60" s="2">
         <v>3.0</v>
       </c>
     </row>
@@ -1248,11 +1254,11 @@
       <c r="A61" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B61" s="2">
+      <c r="B61" s="3">
         <f>9+1/16</f>
         <v>9.0625</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61" s="2">
         <v>3.125</v>
       </c>
     </row>
@@ -1260,10 +1266,10 @@
       <c r="A62" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62" s="2">
         <v>2.75</v>
       </c>
-      <c r="C62" s="2">
+      <c r="C62" s="3">
         <f>9+7/16</f>
         <v>9.4375</v>
       </c>
@@ -1272,11 +1278,11 @@
       <c r="A63" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B63" s="2">
+      <c r="B63" s="3">
         <f>10+9/16</f>
         <v>10.5625</v>
       </c>
-      <c r="C63" s="2">
+      <c r="C63" s="3">
         <f>2+11/16</f>
         <v>2.6875</v>
       </c>
@@ -1285,11 +1291,11 @@
       <c r="A64" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="3">
         <f>4+7/8</f>
         <v>4.875</v>
       </c>
-      <c r="C64" s="2">
+      <c r="C64" s="3">
         <f>3+3/8</f>
         <v>3.375</v>
       </c>
@@ -1298,11 +1304,11 @@
       <c r="A65" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B65" s="2">
-        <f>2+5/8</f>
-        <v>2.625</v>
-      </c>
-      <c r="C65" s="1">
+      <c r="B65" s="3">
+        <f>2+11/16</f>
+        <v>2.6875</v>
+      </c>
+      <c r="C65" s="2">
         <v>9.625</v>
       </c>
     </row>
@@ -1310,11 +1316,11 @@
       <c r="A66" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B66" s="3">
         <f t="shared" ref="B66:B67" si="5">5+5/16</f>
         <v>5.3125</v>
       </c>
-      <c r="C66" s="1">
+      <c r="C66" s="2">
         <v>1.75</v>
       </c>
     </row>
@@ -1322,11 +1328,11 @@
       <c r="A67" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B67" s="2">
+      <c r="B67" s="3">
         <f t="shared" si="5"/>
         <v>5.3125</v>
       </c>
-      <c r="C67" s="1">
+      <c r="C67" s="2">
         <v>1.75</v>
       </c>
     </row>
@@ -1334,10 +1340,10 @@
       <c r="A68" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68" s="2">
         <v>1.75</v>
       </c>
-      <c r="C68" s="2">
+      <c r="C68" s="3">
         <f t="shared" ref="C68:C70" si="6">8+5/8</f>
         <v>8.625</v>
       </c>
@@ -1346,10 +1352,10 @@
       <c r="A69" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69" s="2">
         <v>1.75</v>
       </c>
-      <c r="C69" s="2">
+      <c r="C69" s="3">
         <f t="shared" si="6"/>
         <v>8.625</v>
       </c>
@@ -1358,10 +1364,10 @@
       <c r="A70" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70" s="2">
         <v>1.75</v>
       </c>
-      <c r="C70" s="2">
+      <c r="C70" s="3">
         <f t="shared" si="6"/>
         <v>8.625</v>
       </c>
@@ -1370,10 +1376,10 @@
       <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71" s="2">
         <v>6.125</v>
       </c>
-      <c r="C71" s="2">
+      <c r="C71" s="3">
         <f>4+9/16</f>
         <v>4.5625</v>
       </c>
@@ -1382,11 +1388,11 @@
       <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="2">
+      <c r="B72" s="3">
         <f>10+3/8</f>
         <v>10.375</v>
       </c>
-      <c r="C72" s="1">
+      <c r="C72" s="2">
         <v>2.375</v>
       </c>
     </row>
@@ -1394,10 +1400,10 @@
       <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73" s="2">
         <v>2.5</v>
       </c>
-      <c r="C73" s="1">
+      <c r="C73" s="2">
         <v>10.5</v>
       </c>
     </row>
@@ -1405,10 +1411,10 @@
       <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74" s="2">
         <v>8.5</v>
       </c>
-      <c r="C74" s="2">
+      <c r="C74" s="3">
         <f>2+3/16</f>
         <v>2.1875</v>
       </c>
@@ -1417,10 +1423,10 @@
       <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75" s="2">
         <v>4.0</v>
       </c>
-      <c r="C75" s="1">
+      <c r="C75" s="2">
         <v>9.0</v>
       </c>
     </row>
@@ -1428,11 +1434,11 @@
       <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B76" s="3">
         <f>8+15/16</f>
         <v>8.9375</v>
       </c>
-      <c r="C76" s="2">
+      <c r="C76" s="3">
         <f>2+13/16</f>
         <v>2.8125</v>
       </c>
@@ -1441,10 +1447,10 @@
       <c r="A77" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77" s="2">
         <v>10.5</v>
       </c>
-      <c r="C77" s="1">
+      <c r="C77" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -1452,10 +1458,10 @@
       <c r="A78" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78" s="2">
         <v>5.75</v>
       </c>
-      <c r="C78" s="2">
+      <c r="C78" s="3">
         <f>3+3/8</f>
         <v>3.375</v>
       </c>
@@ -1464,10 +1470,10 @@
       <c r="A79" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79" s="2">
         <v>9.125</v>
       </c>
-      <c r="C79" s="1">
+      <c r="C79" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -1475,11 +1481,11 @@
       <c r="A80" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B80" s="2">
+      <c r="B80" s="3">
         <f> 5 + 13/16</f>
         <v>5.8125</v>
       </c>
-      <c r="C80" s="1">
+      <c r="C80" s="2">
         <v>1.125</v>
       </c>
     </row>
@@ -1487,11 +1493,11 @@
       <c r="A81" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B81" s="2">
+      <c r="B81" s="3">
         <f>7+1/16</f>
         <v>7.0625</v>
       </c>
-      <c r="C81" s="1">
+      <c r="C81" s="2">
         <v>2.0</v>
       </c>
     </row>
@@ -1499,10 +1505,10 @@
       <c r="A82" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82" s="2">
         <v>5.25</v>
       </c>
-      <c r="C82" s="1">
+      <c r="C82" s="2">
         <v>1.5</v>
       </c>
     </row>
@@ -1510,13 +1516,3681 @@
       <c r="A83" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83" s="2">
         <v>8.0</v>
       </c>
-      <c r="C83" s="2">
+      <c r="C83" s="3">
         <f>1+9/16</f>
         <v>1.5625</v>
       </c>
+    </row>
+    <row r="84">
+      <c r="B84" s="3"/>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85">
+      <c r="B85" s="3"/>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86">
+      <c r="B86" s="3"/>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87">
+      <c r="B87" s="3"/>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88">
+      <c r="B88" s="3"/>
+      <c r="C88" s="3"/>
+    </row>
+    <row r="89">
+      <c r="B89" s="3"/>
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90">
+      <c r="B90" s="3"/>
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91">
+      <c r="B91" s="3"/>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92">
+      <c r="B92" s="3"/>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93">
+      <c r="B93" s="3"/>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94">
+      <c r="B94" s="3"/>
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95">
+      <c r="B95" s="3"/>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96">
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+    </row>
+    <row r="97">
+      <c r="B97" s="3"/>
+      <c r="C97" s="3"/>
+    </row>
+    <row r="98">
+      <c r="B98" s="3"/>
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99">
+      <c r="B99" s="3"/>
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100">
+      <c r="B100" s="3"/>
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101">
+      <c r="B101" s="3"/>
+      <c r="C101" s="3"/>
+    </row>
+    <row r="102">
+      <c r="B102" s="3"/>
+      <c r="C102" s="3"/>
+    </row>
+    <row r="103">
+      <c r="B103" s="3"/>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104">
+      <c r="B104" s="3"/>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="105">
+      <c r="B105" s="3"/>
+      <c r="C105" s="3"/>
+    </row>
+    <row r="106">
+      <c r="B106" s="3"/>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107">
+      <c r="B107" s="3"/>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108">
+      <c r="B108" s="3"/>
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109">
+      <c r="B109" s="3"/>
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110">
+      <c r="B110" s="3"/>
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111">
+      <c r="B111" s="3"/>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112">
+      <c r="B112" s="3"/>
+      <c r="C112" s="3"/>
+    </row>
+    <row r="113">
+      <c r="B113" s="3"/>
+      <c r="C113" s="3"/>
+    </row>
+    <row r="114">
+      <c r="B114" s="3"/>
+      <c r="C114" s="3"/>
+    </row>
+    <row r="115">
+      <c r="B115" s="3"/>
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116">
+      <c r="B116" s="3"/>
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117">
+      <c r="B117" s="3"/>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118">
+      <c r="B118" s="3"/>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119">
+      <c r="B119" s="3"/>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120">
+      <c r="B120" s="3"/>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="121">
+      <c r="B121" s="3"/>
+      <c r="C121" s="3"/>
+    </row>
+    <row r="122">
+      <c r="B122" s="3"/>
+      <c r="C122" s="3"/>
+    </row>
+    <row r="123">
+      <c r="B123" s="3"/>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124">
+      <c r="B124" s="3"/>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125">
+      <c r="B125" s="3"/>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126">
+      <c r="B126" s="3"/>
+      <c r="C126" s="3"/>
+    </row>
+    <row r="127">
+      <c r="B127" s="3"/>
+      <c r="C127" s="3"/>
+    </row>
+    <row r="128">
+      <c r="B128" s="3"/>
+      <c r="C128" s="3"/>
+    </row>
+    <row r="129">
+      <c r="B129" s="3"/>
+      <c r="C129" s="3"/>
+    </row>
+    <row r="130">
+      <c r="B130" s="3"/>
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131">
+      <c r="B131" s="3"/>
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132">
+      <c r="B132" s="3"/>
+      <c r="C132" s="3"/>
+    </row>
+    <row r="133">
+      <c r="B133" s="3"/>
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134">
+      <c r="B134" s="3"/>
+      <c r="C134" s="3"/>
+    </row>
+    <row r="135">
+      <c r="B135" s="3"/>
+      <c r="C135" s="3"/>
+    </row>
+    <row r="136">
+      <c r="B136" s="3"/>
+      <c r="C136" s="3"/>
+    </row>
+    <row r="137">
+      <c r="B137" s="3"/>
+      <c r="C137" s="3"/>
+    </row>
+    <row r="138">
+      <c r="B138" s="3"/>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139">
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140">
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141">
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142">
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143">
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144">
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+    </row>
+    <row r="145">
+      <c r="B145" s="3"/>
+      <c r="C145" s="3"/>
+    </row>
+    <row r="146">
+      <c r="B146" s="3"/>
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147">
+      <c r="B147" s="3"/>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148">
+      <c r="B148" s="3"/>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149">
+      <c r="B149" s="3"/>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150">
+      <c r="B150" s="3"/>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151">
+      <c r="B151" s="3"/>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152">
+      <c r="B152" s="3"/>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="153">
+      <c r="B153" s="3"/>
+      <c r="C153" s="3"/>
+    </row>
+    <row r="154">
+      <c r="B154" s="3"/>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155">
+      <c r="B155" s="3"/>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156">
+      <c r="B156" s="3"/>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157">
+      <c r="B157" s="3"/>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158">
+      <c r="B158" s="3"/>
+      <c r="C158" s="3"/>
+    </row>
+    <row r="159">
+      <c r="B159" s="3"/>
+      <c r="C159" s="3"/>
+    </row>
+    <row r="160">
+      <c r="B160" s="3"/>
+      <c r="C160" s="3"/>
+    </row>
+    <row r="161">
+      <c r="B161" s="3"/>
+      <c r="C161" s="3"/>
+    </row>
+    <row r="162">
+      <c r="B162" s="3"/>
+      <c r="C162" s="3"/>
+    </row>
+    <row r="163">
+      <c r="B163" s="3"/>
+      <c r="C163" s="3"/>
+    </row>
+    <row r="164">
+      <c r="B164" s="3"/>
+      <c r="C164" s="3"/>
+    </row>
+    <row r="165">
+      <c r="B165" s="3"/>
+      <c r="C165" s="3"/>
+    </row>
+    <row r="166">
+      <c r="B166" s="3"/>
+      <c r="C166" s="3"/>
+    </row>
+    <row r="167">
+      <c r="B167" s="3"/>
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168">
+      <c r="B168" s="3"/>
+      <c r="C168" s="3"/>
+    </row>
+    <row r="169">
+      <c r="B169" s="3"/>
+      <c r="C169" s="3"/>
+    </row>
+    <row r="170">
+      <c r="B170" s="3"/>
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171">
+      <c r="B171" s="3"/>
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172">
+      <c r="B172" s="3"/>
+      <c r="C172" s="3"/>
+    </row>
+    <row r="173">
+      <c r="B173" s="3"/>
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174">
+      <c r="B174" s="3"/>
+      <c r="C174" s="3"/>
+    </row>
+    <row r="175">
+      <c r="B175" s="3"/>
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176">
+      <c r="B176" s="3"/>
+      <c r="C176" s="3"/>
+    </row>
+    <row r="177">
+      <c r="B177" s="3"/>
+      <c r="C177" s="3"/>
+    </row>
+    <row r="178">
+      <c r="B178" s="3"/>
+      <c r="C178" s="3"/>
+    </row>
+    <row r="179">
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+    </row>
+    <row r="180">
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
+    </row>
+    <row r="181">
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+    </row>
+    <row r="182">
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+    </row>
+    <row r="183">
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+    </row>
+    <row r="184">
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+    </row>
+    <row r="185">
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+    </row>
+    <row r="186">
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+    </row>
+    <row r="187">
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+    </row>
+    <row r="188">
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+    </row>
+    <row r="189">
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+    </row>
+    <row r="190">
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+    </row>
+    <row r="191">
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+    </row>
+    <row r="192">
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+    </row>
+    <row r="193">
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+    </row>
+    <row r="194">
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+    </row>
+    <row r="195">
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+    </row>
+    <row r="196">
+      <c r="B196" s="3"/>
+      <c r="C196" s="3"/>
+    </row>
+    <row r="197">
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+    </row>
+    <row r="198">
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+    </row>
+    <row r="199">
+      <c r="B199" s="3"/>
+      <c r="C199" s="3"/>
+    </row>
+    <row r="200">
+      <c r="B200" s="3"/>
+      <c r="C200" s="3"/>
+    </row>
+    <row r="201">
+      <c r="B201" s="3"/>
+      <c r="C201" s="3"/>
+    </row>
+    <row r="202">
+      <c r="B202" s="3"/>
+      <c r="C202" s="3"/>
+    </row>
+    <row r="203">
+      <c r="B203" s="3"/>
+      <c r="C203" s="3"/>
+    </row>
+    <row r="204">
+      <c r="B204" s="3"/>
+      <c r="C204" s="3"/>
+    </row>
+    <row r="205">
+      <c r="B205" s="3"/>
+      <c r="C205" s="3"/>
+    </row>
+    <row r="206">
+      <c r="B206" s="3"/>
+      <c r="C206" s="3"/>
+    </row>
+    <row r="207">
+      <c r="B207" s="3"/>
+      <c r="C207" s="3"/>
+    </row>
+    <row r="208">
+      <c r="B208" s="3"/>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="209">
+      <c r="B209" s="3"/>
+      <c r="C209" s="3"/>
+    </row>
+    <row r="210">
+      <c r="B210" s="3"/>
+      <c r="C210" s="3"/>
+    </row>
+    <row r="211">
+      <c r="B211" s="3"/>
+      <c r="C211" s="3"/>
+    </row>
+    <row r="212">
+      <c r="B212" s="3"/>
+      <c r="C212" s="3"/>
+    </row>
+    <row r="213">
+      <c r="B213" s="3"/>
+      <c r="C213" s="3"/>
+    </row>
+    <row r="214">
+      <c r="B214" s="3"/>
+      <c r="C214" s="3"/>
+    </row>
+    <row r="215">
+      <c r="B215" s="3"/>
+      <c r="C215" s="3"/>
+    </row>
+    <row r="216">
+      <c r="B216" s="3"/>
+      <c r="C216" s="3"/>
+    </row>
+    <row r="217">
+      <c r="B217" s="3"/>
+      <c r="C217" s="3"/>
+    </row>
+    <row r="218">
+      <c r="B218" s="3"/>
+      <c r="C218" s="3"/>
+    </row>
+    <row r="219">
+      <c r="B219" s="3"/>
+      <c r="C219" s="3"/>
+    </row>
+    <row r="220">
+      <c r="B220" s="3"/>
+      <c r="C220" s="3"/>
+    </row>
+    <row r="221">
+      <c r="B221" s="3"/>
+      <c r="C221" s="3"/>
+    </row>
+    <row r="222">
+      <c r="B222" s="3"/>
+      <c r="C222" s="3"/>
+    </row>
+    <row r="223">
+      <c r="B223" s="3"/>
+      <c r="C223" s="3"/>
+    </row>
+    <row r="224">
+      <c r="B224" s="3"/>
+      <c r="C224" s="3"/>
+    </row>
+    <row r="225">
+      <c r="B225" s="3"/>
+      <c r="C225" s="3"/>
+    </row>
+    <row r="226">
+      <c r="B226" s="3"/>
+      <c r="C226" s="3"/>
+    </row>
+    <row r="227">
+      <c r="B227" s="3"/>
+      <c r="C227" s="3"/>
+    </row>
+    <row r="228">
+      <c r="B228" s="3"/>
+      <c r="C228" s="3"/>
+    </row>
+    <row r="229">
+      <c r="B229" s="3"/>
+      <c r="C229" s="3"/>
+    </row>
+    <row r="230">
+      <c r="B230" s="3"/>
+      <c r="C230" s="3"/>
+    </row>
+    <row r="231">
+      <c r="B231" s="3"/>
+      <c r="C231" s="3"/>
+    </row>
+    <row r="232">
+      <c r="B232" s="3"/>
+      <c r="C232" s="3"/>
+    </row>
+    <row r="233">
+      <c r="B233" s="3"/>
+      <c r="C233" s="3"/>
+    </row>
+    <row r="234">
+      <c r="B234" s="3"/>
+      <c r="C234" s="3"/>
+    </row>
+    <row r="235">
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+    </row>
+    <row r="236">
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+    </row>
+    <row r="237">
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+    </row>
+    <row r="238">
+      <c r="B238" s="3"/>
+      <c r="C238" s="3"/>
+    </row>
+    <row r="239">
+      <c r="B239" s="3"/>
+      <c r="C239" s="3"/>
+    </row>
+    <row r="240">
+      <c r="B240" s="3"/>
+      <c r="C240" s="3"/>
+    </row>
+    <row r="241">
+      <c r="B241" s="3"/>
+      <c r="C241" s="3"/>
+    </row>
+    <row r="242">
+      <c r="B242" s="3"/>
+      <c r="C242" s="3"/>
+    </row>
+    <row r="243">
+      <c r="B243" s="3"/>
+      <c r="C243" s="3"/>
+    </row>
+    <row r="244">
+      <c r="B244" s="3"/>
+      <c r="C244" s="3"/>
+    </row>
+    <row r="245">
+      <c r="B245" s="3"/>
+      <c r="C245" s="3"/>
+    </row>
+    <row r="246">
+      <c r="B246" s="3"/>
+      <c r="C246" s="3"/>
+    </row>
+    <row r="247">
+      <c r="B247" s="3"/>
+      <c r="C247" s="3"/>
+    </row>
+    <row r="248">
+      <c r="B248" s="3"/>
+      <c r="C248" s="3"/>
+    </row>
+    <row r="249">
+      <c r="B249" s="3"/>
+      <c r="C249" s="3"/>
+    </row>
+    <row r="250">
+      <c r="B250" s="3"/>
+      <c r="C250" s="3"/>
+    </row>
+    <row r="251">
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+    </row>
+    <row r="252">
+      <c r="B252" s="3"/>
+      <c r="C252" s="3"/>
+    </row>
+    <row r="253">
+      <c r="B253" s="3"/>
+      <c r="C253" s="3"/>
+    </row>
+    <row r="254">
+      <c r="B254" s="3"/>
+      <c r="C254" s="3"/>
+    </row>
+    <row r="255">
+      <c r="B255" s="3"/>
+      <c r="C255" s="3"/>
+    </row>
+    <row r="256">
+      <c r="B256" s="3"/>
+      <c r="C256" s="3"/>
+    </row>
+    <row r="257">
+      <c r="B257" s="3"/>
+      <c r="C257" s="3"/>
+    </row>
+    <row r="258">
+      <c r="B258" s="3"/>
+      <c r="C258" s="3"/>
+    </row>
+    <row r="259">
+      <c r="B259" s="3"/>
+      <c r="C259" s="3"/>
+    </row>
+    <row r="260">
+      <c r="B260" s="3"/>
+      <c r="C260" s="3"/>
+    </row>
+    <row r="261">
+      <c r="B261" s="3"/>
+      <c r="C261" s="3"/>
+    </row>
+    <row r="262">
+      <c r="B262" s="3"/>
+      <c r="C262" s="3"/>
+    </row>
+    <row r="263">
+      <c r="B263" s="3"/>
+      <c r="C263" s="3"/>
+    </row>
+    <row r="264">
+      <c r="B264" s="3"/>
+      <c r="C264" s="3"/>
+    </row>
+    <row r="265">
+      <c r="B265" s="3"/>
+      <c r="C265" s="3"/>
+    </row>
+    <row r="266">
+      <c r="B266" s="3"/>
+      <c r="C266" s="3"/>
+    </row>
+    <row r="267">
+      <c r="B267" s="3"/>
+      <c r="C267" s="3"/>
+    </row>
+    <row r="268">
+      <c r="B268" s="3"/>
+      <c r="C268" s="3"/>
+    </row>
+    <row r="269">
+      <c r="B269" s="3"/>
+      <c r="C269" s="3"/>
+    </row>
+    <row r="270">
+      <c r="B270" s="3"/>
+      <c r="C270" s="3"/>
+    </row>
+    <row r="271">
+      <c r="B271" s="3"/>
+      <c r="C271" s="3"/>
+    </row>
+    <row r="272">
+      <c r="B272" s="3"/>
+      <c r="C272" s="3"/>
+    </row>
+    <row r="273">
+      <c r="B273" s="3"/>
+      <c r="C273" s="3"/>
+    </row>
+    <row r="274">
+      <c r="B274" s="3"/>
+      <c r="C274" s="3"/>
+    </row>
+    <row r="275">
+      <c r="B275" s="3"/>
+      <c r="C275" s="3"/>
+    </row>
+    <row r="276">
+      <c r="B276" s="3"/>
+      <c r="C276" s="3"/>
+    </row>
+    <row r="277">
+      <c r="B277" s="3"/>
+      <c r="C277" s="3"/>
+    </row>
+    <row r="278">
+      <c r="B278" s="3"/>
+      <c r="C278" s="3"/>
+    </row>
+    <row r="279">
+      <c r="B279" s="3"/>
+      <c r="C279" s="3"/>
+    </row>
+    <row r="280">
+      <c r="B280" s="3"/>
+      <c r="C280" s="3"/>
+    </row>
+    <row r="281">
+      <c r="B281" s="3"/>
+      <c r="C281" s="3"/>
+    </row>
+    <row r="282">
+      <c r="B282" s="3"/>
+      <c r="C282" s="3"/>
+    </row>
+    <row r="283">
+      <c r="B283" s="3"/>
+      <c r="C283" s="3"/>
+    </row>
+    <row r="284">
+      <c r="B284" s="3"/>
+      <c r="C284" s="3"/>
+    </row>
+    <row r="285">
+      <c r="B285" s="3"/>
+      <c r="C285" s="3"/>
+    </row>
+    <row r="286">
+      <c r="B286" s="3"/>
+      <c r="C286" s="3"/>
+    </row>
+    <row r="287">
+      <c r="B287" s="3"/>
+      <c r="C287" s="3"/>
+    </row>
+    <row r="288">
+      <c r="B288" s="3"/>
+      <c r="C288" s="3"/>
+    </row>
+    <row r="289">
+      <c r="B289" s="3"/>
+      <c r="C289" s="3"/>
+    </row>
+    <row r="290">
+      <c r="B290" s="3"/>
+      <c r="C290" s="3"/>
+    </row>
+    <row r="291">
+      <c r="B291" s="3"/>
+      <c r="C291" s="3"/>
+    </row>
+    <row r="292">
+      <c r="B292" s="3"/>
+      <c r="C292" s="3"/>
+    </row>
+    <row r="293">
+      <c r="B293" s="3"/>
+      <c r="C293" s="3"/>
+    </row>
+    <row r="294">
+      <c r="B294" s="3"/>
+      <c r="C294" s="3"/>
+    </row>
+    <row r="295">
+      <c r="B295" s="3"/>
+      <c r="C295" s="3"/>
+    </row>
+    <row r="296">
+      <c r="B296" s="3"/>
+      <c r="C296" s="3"/>
+    </row>
+    <row r="297">
+      <c r="B297" s="3"/>
+      <c r="C297" s="3"/>
+    </row>
+    <row r="298">
+      <c r="B298" s="3"/>
+      <c r="C298" s="3"/>
+    </row>
+    <row r="299">
+      <c r="B299" s="3"/>
+      <c r="C299" s="3"/>
+    </row>
+    <row r="300">
+      <c r="B300" s="3"/>
+      <c r="C300" s="3"/>
+    </row>
+    <row r="301">
+      <c r="B301" s="3"/>
+      <c r="C301" s="3"/>
+    </row>
+    <row r="302">
+      <c r="B302" s="3"/>
+      <c r="C302" s="3"/>
+    </row>
+    <row r="303">
+      <c r="B303" s="3"/>
+      <c r="C303" s="3"/>
+    </row>
+    <row r="304">
+      <c r="B304" s="3"/>
+      <c r="C304" s="3"/>
+    </row>
+    <row r="305">
+      <c r="B305" s="3"/>
+      <c r="C305" s="3"/>
+    </row>
+    <row r="306">
+      <c r="B306" s="3"/>
+      <c r="C306" s="3"/>
+    </row>
+    <row r="307">
+      <c r="B307" s="3"/>
+      <c r="C307" s="3"/>
+    </row>
+    <row r="308">
+      <c r="B308" s="3"/>
+      <c r="C308" s="3"/>
+    </row>
+    <row r="309">
+      <c r="B309" s="3"/>
+      <c r="C309" s="3"/>
+    </row>
+    <row r="310">
+      <c r="B310" s="3"/>
+      <c r="C310" s="3"/>
+    </row>
+    <row r="311">
+      <c r="B311" s="3"/>
+      <c r="C311" s="3"/>
+    </row>
+    <row r="312">
+      <c r="B312" s="3"/>
+      <c r="C312" s="3"/>
+    </row>
+    <row r="313">
+      <c r="B313" s="3"/>
+      <c r="C313" s="3"/>
+    </row>
+    <row r="314">
+      <c r="B314" s="3"/>
+      <c r="C314" s="3"/>
+    </row>
+    <row r="315">
+      <c r="B315" s="3"/>
+      <c r="C315" s="3"/>
+    </row>
+    <row r="316">
+      <c r="B316" s="3"/>
+      <c r="C316" s="3"/>
+    </row>
+    <row r="317">
+      <c r="B317" s="3"/>
+      <c r="C317" s="3"/>
+    </row>
+    <row r="318">
+      <c r="B318" s="3"/>
+      <c r="C318" s="3"/>
+    </row>
+    <row r="319">
+      <c r="B319" s="3"/>
+      <c r="C319" s="3"/>
+    </row>
+    <row r="320">
+      <c r="B320" s="3"/>
+      <c r="C320" s="3"/>
+    </row>
+    <row r="321">
+      <c r="B321" s="3"/>
+      <c r="C321" s="3"/>
+    </row>
+    <row r="322">
+      <c r="B322" s="3"/>
+      <c r="C322" s="3"/>
+    </row>
+    <row r="323">
+      <c r="B323" s="3"/>
+      <c r="C323" s="3"/>
+    </row>
+    <row r="324">
+      <c r="B324" s="3"/>
+      <c r="C324" s="3"/>
+    </row>
+    <row r="325">
+      <c r="B325" s="3"/>
+      <c r="C325" s="3"/>
+    </row>
+    <row r="326">
+      <c r="B326" s="3"/>
+      <c r="C326" s="3"/>
+    </row>
+    <row r="327">
+      <c r="B327" s="3"/>
+      <c r="C327" s="3"/>
+    </row>
+    <row r="328">
+      <c r="B328" s="3"/>
+      <c r="C328" s="3"/>
+    </row>
+    <row r="329">
+      <c r="B329" s="3"/>
+      <c r="C329" s="3"/>
+    </row>
+    <row r="330">
+      <c r="B330" s="3"/>
+      <c r="C330" s="3"/>
+    </row>
+    <row r="331">
+      <c r="B331" s="3"/>
+      <c r="C331" s="3"/>
+    </row>
+    <row r="332">
+      <c r="B332" s="3"/>
+      <c r="C332" s="3"/>
+    </row>
+    <row r="333">
+      <c r="B333" s="3"/>
+      <c r="C333" s="3"/>
+    </row>
+    <row r="334">
+      <c r="B334" s="3"/>
+      <c r="C334" s="3"/>
+    </row>
+    <row r="335">
+      <c r="B335" s="3"/>
+      <c r="C335" s="3"/>
+    </row>
+    <row r="336">
+      <c r="B336" s="3"/>
+      <c r="C336" s="3"/>
+    </row>
+    <row r="337">
+      <c r="B337" s="3"/>
+      <c r="C337" s="3"/>
+    </row>
+    <row r="338">
+      <c r="B338" s="3"/>
+      <c r="C338" s="3"/>
+    </row>
+    <row r="339">
+      <c r="B339" s="3"/>
+      <c r="C339" s="3"/>
+    </row>
+    <row r="340">
+      <c r="B340" s="3"/>
+      <c r="C340" s="3"/>
+    </row>
+    <row r="341">
+      <c r="B341" s="3"/>
+      <c r="C341" s="3"/>
+    </row>
+    <row r="342">
+      <c r="B342" s="3"/>
+      <c r="C342" s="3"/>
+    </row>
+    <row r="343">
+      <c r="B343" s="3"/>
+      <c r="C343" s="3"/>
+    </row>
+    <row r="344">
+      <c r="B344" s="3"/>
+      <c r="C344" s="3"/>
+    </row>
+    <row r="345">
+      <c r="B345" s="3"/>
+      <c r="C345" s="3"/>
+    </row>
+    <row r="346">
+      <c r="B346" s="3"/>
+      <c r="C346" s="3"/>
+    </row>
+    <row r="347">
+      <c r="B347" s="3"/>
+      <c r="C347" s="3"/>
+    </row>
+    <row r="348">
+      <c r="B348" s="3"/>
+      <c r="C348" s="3"/>
+    </row>
+    <row r="349">
+      <c r="B349" s="3"/>
+      <c r="C349" s="3"/>
+    </row>
+    <row r="350">
+      <c r="B350" s="3"/>
+      <c r="C350" s="3"/>
+    </row>
+    <row r="351">
+      <c r="B351" s="3"/>
+      <c r="C351" s="3"/>
+    </row>
+    <row r="352">
+      <c r="B352" s="3"/>
+      <c r="C352" s="3"/>
+    </row>
+    <row r="353">
+      <c r="B353" s="3"/>
+      <c r="C353" s="3"/>
+    </row>
+    <row r="354">
+      <c r="B354" s="3"/>
+      <c r="C354" s="3"/>
+    </row>
+    <row r="355">
+      <c r="B355" s="3"/>
+      <c r="C355" s="3"/>
+    </row>
+    <row r="356">
+      <c r="B356" s="3"/>
+      <c r="C356" s="3"/>
+    </row>
+    <row r="357">
+      <c r="B357" s="3"/>
+      <c r="C357" s="3"/>
+    </row>
+    <row r="358">
+      <c r="B358" s="3"/>
+      <c r="C358" s="3"/>
+    </row>
+    <row r="359">
+      <c r="B359" s="3"/>
+      <c r="C359" s="3"/>
+    </row>
+    <row r="360">
+      <c r="B360" s="3"/>
+      <c r="C360" s="3"/>
+    </row>
+    <row r="361">
+      <c r="B361" s="3"/>
+      <c r="C361" s="3"/>
+    </row>
+    <row r="362">
+      <c r="B362" s="3"/>
+      <c r="C362" s="3"/>
+    </row>
+    <row r="363">
+      <c r="B363" s="3"/>
+      <c r="C363" s="3"/>
+    </row>
+    <row r="364">
+      <c r="B364" s="3"/>
+      <c r="C364" s="3"/>
+    </row>
+    <row r="365">
+      <c r="B365" s="3"/>
+      <c r="C365" s="3"/>
+    </row>
+    <row r="366">
+      <c r="B366" s="3"/>
+      <c r="C366" s="3"/>
+    </row>
+    <row r="367">
+      <c r="B367" s="3"/>
+      <c r="C367" s="3"/>
+    </row>
+    <row r="368">
+      <c r="B368" s="3"/>
+      <c r="C368" s="3"/>
+    </row>
+    <row r="369">
+      <c r="B369" s="3"/>
+      <c r="C369" s="3"/>
+    </row>
+    <row r="370">
+      <c r="B370" s="3"/>
+      <c r="C370" s="3"/>
+    </row>
+    <row r="371">
+      <c r="B371" s="3"/>
+      <c r="C371" s="3"/>
+    </row>
+    <row r="372">
+      <c r="B372" s="3"/>
+      <c r="C372" s="3"/>
+    </row>
+    <row r="373">
+      <c r="B373" s="3"/>
+      <c r="C373" s="3"/>
+    </row>
+    <row r="374">
+      <c r="B374" s="3"/>
+      <c r="C374" s="3"/>
+    </row>
+    <row r="375">
+      <c r="B375" s="3"/>
+      <c r="C375" s="3"/>
+    </row>
+    <row r="376">
+      <c r="B376" s="3"/>
+      <c r="C376" s="3"/>
+    </row>
+    <row r="377">
+      <c r="B377" s="3"/>
+      <c r="C377" s="3"/>
+    </row>
+    <row r="378">
+      <c r="B378" s="3"/>
+      <c r="C378" s="3"/>
+    </row>
+    <row r="379">
+      <c r="B379" s="3"/>
+      <c r="C379" s="3"/>
+    </row>
+    <row r="380">
+      <c r="B380" s="3"/>
+      <c r="C380" s="3"/>
+    </row>
+    <row r="381">
+      <c r="B381" s="3"/>
+      <c r="C381" s="3"/>
+    </row>
+    <row r="382">
+      <c r="B382" s="3"/>
+      <c r="C382" s="3"/>
+    </row>
+    <row r="383">
+      <c r="B383" s="3"/>
+      <c r="C383" s="3"/>
+    </row>
+    <row r="384">
+      <c r="B384" s="3"/>
+      <c r="C384" s="3"/>
+    </row>
+    <row r="385">
+      <c r="B385" s="3"/>
+      <c r="C385" s="3"/>
+    </row>
+    <row r="386">
+      <c r="B386" s="3"/>
+      <c r="C386" s="3"/>
+    </row>
+    <row r="387">
+      <c r="B387" s="3"/>
+      <c r="C387" s="3"/>
+    </row>
+    <row r="388">
+      <c r="B388" s="3"/>
+      <c r="C388" s="3"/>
+    </row>
+    <row r="389">
+      <c r="B389" s="3"/>
+      <c r="C389" s="3"/>
+    </row>
+    <row r="390">
+      <c r="B390" s="3"/>
+      <c r="C390" s="3"/>
+    </row>
+    <row r="391">
+      <c r="B391" s="3"/>
+      <c r="C391" s="3"/>
+    </row>
+    <row r="392">
+      <c r="B392" s="3"/>
+      <c r="C392" s="3"/>
+    </row>
+    <row r="393">
+      <c r="B393" s="3"/>
+      <c r="C393" s="3"/>
+    </row>
+    <row r="394">
+      <c r="B394" s="3"/>
+      <c r="C394" s="3"/>
+    </row>
+    <row r="395">
+      <c r="B395" s="3"/>
+      <c r="C395" s="3"/>
+    </row>
+    <row r="396">
+      <c r="B396" s="3"/>
+      <c r="C396" s="3"/>
+    </row>
+    <row r="397">
+      <c r="B397" s="3"/>
+      <c r="C397" s="3"/>
+    </row>
+    <row r="398">
+      <c r="B398" s="3"/>
+      <c r="C398" s="3"/>
+    </row>
+    <row r="399">
+      <c r="B399" s="3"/>
+      <c r="C399" s="3"/>
+    </row>
+    <row r="400">
+      <c r="B400" s="3"/>
+      <c r="C400" s="3"/>
+    </row>
+    <row r="401">
+      <c r="B401" s="3"/>
+      <c r="C401" s="3"/>
+    </row>
+    <row r="402">
+      <c r="B402" s="3"/>
+      <c r="C402" s="3"/>
+    </row>
+    <row r="403">
+      <c r="B403" s="3"/>
+      <c r="C403" s="3"/>
+    </row>
+    <row r="404">
+      <c r="B404" s="3"/>
+      <c r="C404" s="3"/>
+    </row>
+    <row r="405">
+      <c r="B405" s="3"/>
+      <c r="C405" s="3"/>
+    </row>
+    <row r="406">
+      <c r="B406" s="3"/>
+      <c r="C406" s="3"/>
+    </row>
+    <row r="407">
+      <c r="B407" s="3"/>
+      <c r="C407" s="3"/>
+    </row>
+    <row r="408">
+      <c r="B408" s="3"/>
+      <c r="C408" s="3"/>
+    </row>
+    <row r="409">
+      <c r="B409" s="3"/>
+      <c r="C409" s="3"/>
+    </row>
+    <row r="410">
+      <c r="B410" s="3"/>
+      <c r="C410" s="3"/>
+    </row>
+    <row r="411">
+      <c r="B411" s="3"/>
+      <c r="C411" s="3"/>
+    </row>
+    <row r="412">
+      <c r="B412" s="3"/>
+      <c r="C412" s="3"/>
+    </row>
+    <row r="413">
+      <c r="B413" s="3"/>
+      <c r="C413" s="3"/>
+    </row>
+    <row r="414">
+      <c r="B414" s="3"/>
+      <c r="C414" s="3"/>
+    </row>
+    <row r="415">
+      <c r="B415" s="3"/>
+      <c r="C415" s="3"/>
+    </row>
+    <row r="416">
+      <c r="B416" s="3"/>
+      <c r="C416" s="3"/>
+    </row>
+    <row r="417">
+      <c r="B417" s="3"/>
+      <c r="C417" s="3"/>
+    </row>
+    <row r="418">
+      <c r="B418" s="3"/>
+      <c r="C418" s="3"/>
+    </row>
+    <row r="419">
+      <c r="B419" s="3"/>
+      <c r="C419" s="3"/>
+    </row>
+    <row r="420">
+      <c r="B420" s="3"/>
+      <c r="C420" s="3"/>
+    </row>
+    <row r="421">
+      <c r="B421" s="3"/>
+      <c r="C421" s="3"/>
+    </row>
+    <row r="422">
+      <c r="B422" s="3"/>
+      <c r="C422" s="3"/>
+    </row>
+    <row r="423">
+      <c r="B423" s="3"/>
+      <c r="C423" s="3"/>
+    </row>
+    <row r="424">
+      <c r="B424" s="3"/>
+      <c r="C424" s="3"/>
+    </row>
+    <row r="425">
+      <c r="B425" s="3"/>
+      <c r="C425" s="3"/>
+    </row>
+    <row r="426">
+      <c r="B426" s="3"/>
+      <c r="C426" s="3"/>
+    </row>
+    <row r="427">
+      <c r="B427" s="3"/>
+      <c r="C427" s="3"/>
+    </row>
+    <row r="428">
+      <c r="B428" s="3"/>
+      <c r="C428" s="3"/>
+    </row>
+    <row r="429">
+      <c r="B429" s="3"/>
+      <c r="C429" s="3"/>
+    </row>
+    <row r="430">
+      <c r="B430" s="3"/>
+      <c r="C430" s="3"/>
+    </row>
+    <row r="431">
+      <c r="B431" s="3"/>
+      <c r="C431" s="3"/>
+    </row>
+    <row r="432">
+      <c r="B432" s="3"/>
+      <c r="C432" s="3"/>
+    </row>
+    <row r="433">
+      <c r="B433" s="3"/>
+      <c r="C433" s="3"/>
+    </row>
+    <row r="434">
+      <c r="B434" s="3"/>
+      <c r="C434" s="3"/>
+    </row>
+    <row r="435">
+      <c r="B435" s="3"/>
+      <c r="C435" s="3"/>
+    </row>
+    <row r="436">
+      <c r="B436" s="3"/>
+      <c r="C436" s="3"/>
+    </row>
+    <row r="437">
+      <c r="B437" s="3"/>
+      <c r="C437" s="3"/>
+    </row>
+    <row r="438">
+      <c r="B438" s="3"/>
+      <c r="C438" s="3"/>
+    </row>
+    <row r="439">
+      <c r="B439" s="3"/>
+      <c r="C439" s="3"/>
+    </row>
+    <row r="440">
+      <c r="B440" s="3"/>
+      <c r="C440" s="3"/>
+    </row>
+    <row r="441">
+      <c r="B441" s="3"/>
+      <c r="C441" s="3"/>
+    </row>
+    <row r="442">
+      <c r="B442" s="3"/>
+      <c r="C442" s="3"/>
+    </row>
+    <row r="443">
+      <c r="B443" s="3"/>
+      <c r="C443" s="3"/>
+    </row>
+    <row r="444">
+      <c r="B444" s="3"/>
+      <c r="C444" s="3"/>
+    </row>
+    <row r="445">
+      <c r="B445" s="3"/>
+      <c r="C445" s="3"/>
+    </row>
+    <row r="446">
+      <c r="B446" s="3"/>
+      <c r="C446" s="3"/>
+    </row>
+    <row r="447">
+      <c r="B447" s="3"/>
+      <c r="C447" s="3"/>
+    </row>
+    <row r="448">
+      <c r="B448" s="3"/>
+      <c r="C448" s="3"/>
+    </row>
+    <row r="449">
+      <c r="B449" s="3"/>
+      <c r="C449" s="3"/>
+    </row>
+    <row r="450">
+      <c r="B450" s="3"/>
+      <c r="C450" s="3"/>
+    </row>
+    <row r="451">
+      <c r="B451" s="3"/>
+      <c r="C451" s="3"/>
+    </row>
+    <row r="452">
+      <c r="B452" s="3"/>
+      <c r="C452" s="3"/>
+    </row>
+    <row r="453">
+      <c r="B453" s="3"/>
+      <c r="C453" s="3"/>
+    </row>
+    <row r="454">
+      <c r="B454" s="3"/>
+      <c r="C454" s="3"/>
+    </row>
+    <row r="455">
+      <c r="B455" s="3"/>
+      <c r="C455" s="3"/>
+    </row>
+    <row r="456">
+      <c r="B456" s="3"/>
+      <c r="C456" s="3"/>
+    </row>
+    <row r="457">
+      <c r="B457" s="3"/>
+      <c r="C457" s="3"/>
+    </row>
+    <row r="458">
+      <c r="B458" s="3"/>
+      <c r="C458" s="3"/>
+    </row>
+    <row r="459">
+      <c r="B459" s="3"/>
+      <c r="C459" s="3"/>
+    </row>
+    <row r="460">
+      <c r="B460" s="3"/>
+      <c r="C460" s="3"/>
+    </row>
+    <row r="461">
+      <c r="B461" s="3"/>
+      <c r="C461" s="3"/>
+    </row>
+    <row r="462">
+      <c r="B462" s="3"/>
+      <c r="C462" s="3"/>
+    </row>
+    <row r="463">
+      <c r="B463" s="3"/>
+      <c r="C463" s="3"/>
+    </row>
+    <row r="464">
+      <c r="B464" s="3"/>
+      <c r="C464" s="3"/>
+    </row>
+    <row r="465">
+      <c r="B465" s="3"/>
+      <c r="C465" s="3"/>
+    </row>
+    <row r="466">
+      <c r="B466" s="3"/>
+      <c r="C466" s="3"/>
+    </row>
+    <row r="467">
+      <c r="B467" s="3"/>
+      <c r="C467" s="3"/>
+    </row>
+    <row r="468">
+      <c r="B468" s="3"/>
+      <c r="C468" s="3"/>
+    </row>
+    <row r="469">
+      <c r="B469" s="3"/>
+      <c r="C469" s="3"/>
+    </row>
+    <row r="470">
+      <c r="B470" s="3"/>
+      <c r="C470" s="3"/>
+    </row>
+    <row r="471">
+      <c r="B471" s="3"/>
+      <c r="C471" s="3"/>
+    </row>
+    <row r="472">
+      <c r="B472" s="3"/>
+      <c r="C472" s="3"/>
+    </row>
+    <row r="473">
+      <c r="B473" s="3"/>
+      <c r="C473" s="3"/>
+    </row>
+    <row r="474">
+      <c r="B474" s="3"/>
+      <c r="C474" s="3"/>
+    </row>
+    <row r="475">
+      <c r="B475" s="3"/>
+      <c r="C475" s="3"/>
+    </row>
+    <row r="476">
+      <c r="B476" s="3"/>
+      <c r="C476" s="3"/>
+    </row>
+    <row r="477">
+      <c r="B477" s="3"/>
+      <c r="C477" s="3"/>
+    </row>
+    <row r="478">
+      <c r="B478" s="3"/>
+      <c r="C478" s="3"/>
+    </row>
+    <row r="479">
+      <c r="B479" s="3"/>
+      <c r="C479" s="3"/>
+    </row>
+    <row r="480">
+      <c r="B480" s="3"/>
+      <c r="C480" s="3"/>
+    </row>
+    <row r="481">
+      <c r="B481" s="3"/>
+      <c r="C481" s="3"/>
+    </row>
+    <row r="482">
+      <c r="B482" s="3"/>
+      <c r="C482" s="3"/>
+    </row>
+    <row r="483">
+      <c r="B483" s="3"/>
+      <c r="C483" s="3"/>
+    </row>
+    <row r="484">
+      <c r="B484" s="3"/>
+      <c r="C484" s="3"/>
+    </row>
+    <row r="485">
+      <c r="B485" s="3"/>
+      <c r="C485" s="3"/>
+    </row>
+    <row r="486">
+      <c r="B486" s="3"/>
+      <c r="C486" s="3"/>
+    </row>
+    <row r="487">
+      <c r="B487" s="3"/>
+      <c r="C487" s="3"/>
+    </row>
+    <row r="488">
+      <c r="B488" s="3"/>
+      <c r="C488" s="3"/>
+    </row>
+    <row r="489">
+      <c r="B489" s="3"/>
+      <c r="C489" s="3"/>
+    </row>
+    <row r="490">
+      <c r="B490" s="3"/>
+      <c r="C490" s="3"/>
+    </row>
+    <row r="491">
+      <c r="B491" s="3"/>
+      <c r="C491" s="3"/>
+    </row>
+    <row r="492">
+      <c r="B492" s="3"/>
+      <c r="C492" s="3"/>
+    </row>
+    <row r="493">
+      <c r="B493" s="3"/>
+      <c r="C493" s="3"/>
+    </row>
+    <row r="494">
+      <c r="B494" s="3"/>
+      <c r="C494" s="3"/>
+    </row>
+    <row r="495">
+      <c r="B495" s="3"/>
+      <c r="C495" s="3"/>
+    </row>
+    <row r="496">
+      <c r="B496" s="3"/>
+      <c r="C496" s="3"/>
+    </row>
+    <row r="497">
+      <c r="B497" s="3"/>
+      <c r="C497" s="3"/>
+    </row>
+    <row r="498">
+      <c r="B498" s="3"/>
+      <c r="C498" s="3"/>
+    </row>
+    <row r="499">
+      <c r="B499" s="3"/>
+      <c r="C499" s="3"/>
+    </row>
+    <row r="500">
+      <c r="B500" s="3"/>
+      <c r="C500" s="3"/>
+    </row>
+    <row r="501">
+      <c r="B501" s="3"/>
+      <c r="C501" s="3"/>
+    </row>
+    <row r="502">
+      <c r="B502" s="3"/>
+      <c r="C502" s="3"/>
+    </row>
+    <row r="503">
+      <c r="B503" s="3"/>
+      <c r="C503" s="3"/>
+    </row>
+    <row r="504">
+      <c r="B504" s="3"/>
+      <c r="C504" s="3"/>
+    </row>
+    <row r="505">
+      <c r="B505" s="3"/>
+      <c r="C505" s="3"/>
+    </row>
+    <row r="506">
+      <c r="B506" s="3"/>
+      <c r="C506" s="3"/>
+    </row>
+    <row r="507">
+      <c r="B507" s="3"/>
+      <c r="C507" s="3"/>
+    </row>
+    <row r="508">
+      <c r="B508" s="3"/>
+      <c r="C508" s="3"/>
+    </row>
+    <row r="509">
+      <c r="B509" s="3"/>
+      <c r="C509" s="3"/>
+    </row>
+    <row r="510">
+      <c r="B510" s="3"/>
+      <c r="C510" s="3"/>
+    </row>
+    <row r="511">
+      <c r="B511" s="3"/>
+      <c r="C511" s="3"/>
+    </row>
+    <row r="512">
+      <c r="B512" s="3"/>
+      <c r="C512" s="3"/>
+    </row>
+    <row r="513">
+      <c r="B513" s="3"/>
+      <c r="C513" s="3"/>
+    </row>
+    <row r="514">
+      <c r="B514" s="3"/>
+      <c r="C514" s="3"/>
+    </row>
+    <row r="515">
+      <c r="B515" s="3"/>
+      <c r="C515" s="3"/>
+    </row>
+    <row r="516">
+      <c r="B516" s="3"/>
+      <c r="C516" s="3"/>
+    </row>
+    <row r="517">
+      <c r="B517" s="3"/>
+      <c r="C517" s="3"/>
+    </row>
+    <row r="518">
+      <c r="B518" s="3"/>
+      <c r="C518" s="3"/>
+    </row>
+    <row r="519">
+      <c r="B519" s="3"/>
+      <c r="C519" s="3"/>
+    </row>
+    <row r="520">
+      <c r="B520" s="3"/>
+      <c r="C520" s="3"/>
+    </row>
+    <row r="521">
+      <c r="B521" s="3"/>
+      <c r="C521" s="3"/>
+    </row>
+    <row r="522">
+      <c r="B522" s="3"/>
+      <c r="C522" s="3"/>
+    </row>
+    <row r="523">
+      <c r="B523" s="3"/>
+      <c r="C523" s="3"/>
+    </row>
+    <row r="524">
+      <c r="B524" s="3"/>
+      <c r="C524" s="3"/>
+    </row>
+    <row r="525">
+      <c r="B525" s="3"/>
+      <c r="C525" s="3"/>
+    </row>
+    <row r="526">
+      <c r="B526" s="3"/>
+      <c r="C526" s="3"/>
+    </row>
+    <row r="527">
+      <c r="B527" s="3"/>
+      <c r="C527" s="3"/>
+    </row>
+    <row r="528">
+      <c r="B528" s="3"/>
+      <c r="C528" s="3"/>
+    </row>
+    <row r="529">
+      <c r="B529" s="3"/>
+      <c r="C529" s="3"/>
+    </row>
+    <row r="530">
+      <c r="B530" s="3"/>
+      <c r="C530" s="3"/>
+    </row>
+    <row r="531">
+      <c r="B531" s="3"/>
+      <c r="C531" s="3"/>
+    </row>
+    <row r="532">
+      <c r="B532" s="3"/>
+      <c r="C532" s="3"/>
+    </row>
+    <row r="533">
+      <c r="B533" s="3"/>
+      <c r="C533" s="3"/>
+    </row>
+    <row r="534">
+      <c r="B534" s="3"/>
+      <c r="C534" s="3"/>
+    </row>
+    <row r="535">
+      <c r="B535" s="3"/>
+      <c r="C535" s="3"/>
+    </row>
+    <row r="536">
+      <c r="B536" s="3"/>
+      <c r="C536" s="3"/>
+    </row>
+    <row r="537">
+      <c r="B537" s="3"/>
+      <c r="C537" s="3"/>
+    </row>
+    <row r="538">
+      <c r="B538" s="3"/>
+      <c r="C538" s="3"/>
+    </row>
+    <row r="539">
+      <c r="B539" s="3"/>
+      <c r="C539" s="3"/>
+    </row>
+    <row r="540">
+      <c r="B540" s="3"/>
+      <c r="C540" s="3"/>
+    </row>
+    <row r="541">
+      <c r="B541" s="3"/>
+      <c r="C541" s="3"/>
+    </row>
+    <row r="542">
+      <c r="B542" s="3"/>
+      <c r="C542" s="3"/>
+    </row>
+    <row r="543">
+      <c r="B543" s="3"/>
+      <c r="C543" s="3"/>
+    </row>
+    <row r="544">
+      <c r="B544" s="3"/>
+      <c r="C544" s="3"/>
+    </row>
+    <row r="545">
+      <c r="B545" s="3"/>
+      <c r="C545" s="3"/>
+    </row>
+    <row r="546">
+      <c r="B546" s="3"/>
+      <c r="C546" s="3"/>
+    </row>
+    <row r="547">
+      <c r="B547" s="3"/>
+      <c r="C547" s="3"/>
+    </row>
+    <row r="548">
+      <c r="B548" s="3"/>
+      <c r="C548" s="3"/>
+    </row>
+    <row r="549">
+      <c r="B549" s="3"/>
+      <c r="C549" s="3"/>
+    </row>
+    <row r="550">
+      <c r="B550" s="3"/>
+      <c r="C550" s="3"/>
+    </row>
+    <row r="551">
+      <c r="B551" s="3"/>
+      <c r="C551" s="3"/>
+    </row>
+    <row r="552">
+      <c r="B552" s="3"/>
+      <c r="C552" s="3"/>
+    </row>
+    <row r="553">
+      <c r="B553" s="3"/>
+      <c r="C553" s="3"/>
+    </row>
+    <row r="554">
+      <c r="B554" s="3"/>
+      <c r="C554" s="3"/>
+    </row>
+    <row r="555">
+      <c r="B555" s="3"/>
+      <c r="C555" s="3"/>
+    </row>
+    <row r="556">
+      <c r="B556" s="3"/>
+      <c r="C556" s="3"/>
+    </row>
+    <row r="557">
+      <c r="B557" s="3"/>
+      <c r="C557" s="3"/>
+    </row>
+    <row r="558">
+      <c r="B558" s="3"/>
+      <c r="C558" s="3"/>
+    </row>
+    <row r="559">
+      <c r="B559" s="3"/>
+      <c r="C559" s="3"/>
+    </row>
+    <row r="560">
+      <c r="B560" s="3"/>
+      <c r="C560" s="3"/>
+    </row>
+    <row r="561">
+      <c r="B561" s="3"/>
+      <c r="C561" s="3"/>
+    </row>
+    <row r="562">
+      <c r="B562" s="3"/>
+      <c r="C562" s="3"/>
+    </row>
+    <row r="563">
+      <c r="B563" s="3"/>
+      <c r="C563" s="3"/>
+    </row>
+    <row r="564">
+      <c r="B564" s="3"/>
+      <c r="C564" s="3"/>
+    </row>
+    <row r="565">
+      <c r="B565" s="3"/>
+      <c r="C565" s="3"/>
+    </row>
+    <row r="566">
+      <c r="B566" s="3"/>
+      <c r="C566" s="3"/>
+    </row>
+    <row r="567">
+      <c r="B567" s="3"/>
+      <c r="C567" s="3"/>
+    </row>
+    <row r="568">
+      <c r="B568" s="3"/>
+      <c r="C568" s="3"/>
+    </row>
+    <row r="569">
+      <c r="B569" s="3"/>
+      <c r="C569" s="3"/>
+    </row>
+    <row r="570">
+      <c r="B570" s="3"/>
+      <c r="C570" s="3"/>
+    </row>
+    <row r="571">
+      <c r="B571" s="3"/>
+      <c r="C571" s="3"/>
+    </row>
+    <row r="572">
+      <c r="B572" s="3"/>
+      <c r="C572" s="3"/>
+    </row>
+    <row r="573">
+      <c r="B573" s="3"/>
+      <c r="C573" s="3"/>
+    </row>
+    <row r="574">
+      <c r="B574" s="3"/>
+      <c r="C574" s="3"/>
+    </row>
+    <row r="575">
+      <c r="B575" s="3"/>
+      <c r="C575" s="3"/>
+    </row>
+    <row r="576">
+      <c r="B576" s="3"/>
+      <c r="C576" s="3"/>
+    </row>
+    <row r="577">
+      <c r="B577" s="3"/>
+      <c r="C577" s="3"/>
+    </row>
+    <row r="578">
+      <c r="B578" s="3"/>
+      <c r="C578" s="3"/>
+    </row>
+    <row r="579">
+      <c r="B579" s="3"/>
+      <c r="C579" s="3"/>
+    </row>
+    <row r="580">
+      <c r="B580" s="3"/>
+      <c r="C580" s="3"/>
+    </row>
+    <row r="581">
+      <c r="B581" s="3"/>
+      <c r="C581" s="3"/>
+    </row>
+    <row r="582">
+      <c r="B582" s="3"/>
+      <c r="C582" s="3"/>
+    </row>
+    <row r="583">
+      <c r="B583" s="3"/>
+      <c r="C583" s="3"/>
+    </row>
+    <row r="584">
+      <c r="B584" s="3"/>
+      <c r="C584" s="3"/>
+    </row>
+    <row r="585">
+      <c r="B585" s="3"/>
+      <c r="C585" s="3"/>
+    </row>
+    <row r="586">
+      <c r="B586" s="3"/>
+      <c r="C586" s="3"/>
+    </row>
+    <row r="587">
+      <c r="B587" s="3"/>
+      <c r="C587" s="3"/>
+    </row>
+    <row r="588">
+      <c r="B588" s="3"/>
+      <c r="C588" s="3"/>
+    </row>
+    <row r="589">
+      <c r="B589" s="3"/>
+      <c r="C589" s="3"/>
+    </row>
+    <row r="590">
+      <c r="B590" s="3"/>
+      <c r="C590" s="3"/>
+    </row>
+    <row r="591">
+      <c r="B591" s="3"/>
+      <c r="C591" s="3"/>
+    </row>
+    <row r="592">
+      <c r="B592" s="3"/>
+      <c r="C592" s="3"/>
+    </row>
+    <row r="593">
+      <c r="B593" s="3"/>
+      <c r="C593" s="3"/>
+    </row>
+    <row r="594">
+      <c r="B594" s="3"/>
+      <c r="C594" s="3"/>
+    </row>
+    <row r="595">
+      <c r="B595" s="3"/>
+      <c r="C595" s="3"/>
+    </row>
+    <row r="596">
+      <c r="B596" s="3"/>
+      <c r="C596" s="3"/>
+    </row>
+    <row r="597">
+      <c r="B597" s="3"/>
+      <c r="C597" s="3"/>
+    </row>
+    <row r="598">
+      <c r="B598" s="3"/>
+      <c r="C598" s="3"/>
+    </row>
+    <row r="599">
+      <c r="B599" s="3"/>
+      <c r="C599" s="3"/>
+    </row>
+    <row r="600">
+      <c r="B600" s="3"/>
+      <c r="C600" s="3"/>
+    </row>
+    <row r="601">
+      <c r="B601" s="3"/>
+      <c r="C601" s="3"/>
+    </row>
+    <row r="602">
+      <c r="B602" s="3"/>
+      <c r="C602" s="3"/>
+    </row>
+    <row r="603">
+      <c r="B603" s="3"/>
+      <c r="C603" s="3"/>
+    </row>
+    <row r="604">
+      <c r="B604" s="3"/>
+      <c r="C604" s="3"/>
+    </row>
+    <row r="605">
+      <c r="B605" s="3"/>
+      <c r="C605" s="3"/>
+    </row>
+    <row r="606">
+      <c r="B606" s="3"/>
+      <c r="C606" s="3"/>
+    </row>
+    <row r="607">
+      <c r="B607" s="3"/>
+      <c r="C607" s="3"/>
+    </row>
+    <row r="608">
+      <c r="B608" s="3"/>
+      <c r="C608" s="3"/>
+    </row>
+    <row r="609">
+      <c r="B609" s="3"/>
+      <c r="C609" s="3"/>
+    </row>
+    <row r="610">
+      <c r="B610" s="3"/>
+      <c r="C610" s="3"/>
+    </row>
+    <row r="611">
+      <c r="B611" s="3"/>
+      <c r="C611" s="3"/>
+    </row>
+    <row r="612">
+      <c r="B612" s="3"/>
+      <c r="C612" s="3"/>
+    </row>
+    <row r="613">
+      <c r="B613" s="3"/>
+      <c r="C613" s="3"/>
+    </row>
+    <row r="614">
+      <c r="B614" s="3"/>
+      <c r="C614" s="3"/>
+    </row>
+    <row r="615">
+      <c r="B615" s="3"/>
+      <c r="C615" s="3"/>
+    </row>
+    <row r="616">
+      <c r="B616" s="3"/>
+      <c r="C616" s="3"/>
+    </row>
+    <row r="617">
+      <c r="B617" s="3"/>
+      <c r="C617" s="3"/>
+    </row>
+    <row r="618">
+      <c r="B618" s="3"/>
+      <c r="C618" s="3"/>
+    </row>
+    <row r="619">
+      <c r="B619" s="3"/>
+      <c r="C619" s="3"/>
+    </row>
+    <row r="620">
+      <c r="B620" s="3"/>
+      <c r="C620" s="3"/>
+    </row>
+    <row r="621">
+      <c r="B621" s="3"/>
+      <c r="C621" s="3"/>
+    </row>
+    <row r="622">
+      <c r="B622" s="3"/>
+      <c r="C622" s="3"/>
+    </row>
+    <row r="623">
+      <c r="B623" s="3"/>
+      <c r="C623" s="3"/>
+    </row>
+    <row r="624">
+      <c r="B624" s="3"/>
+      <c r="C624" s="3"/>
+    </row>
+    <row r="625">
+      <c r="B625" s="3"/>
+      <c r="C625" s="3"/>
+    </row>
+    <row r="626">
+      <c r="B626" s="3"/>
+      <c r="C626" s="3"/>
+    </row>
+    <row r="627">
+      <c r="B627" s="3"/>
+      <c r="C627" s="3"/>
+    </row>
+    <row r="628">
+      <c r="B628" s="3"/>
+      <c r="C628" s="3"/>
+    </row>
+    <row r="629">
+      <c r="B629" s="3"/>
+      <c r="C629" s="3"/>
+    </row>
+    <row r="630">
+      <c r="B630" s="3"/>
+      <c r="C630" s="3"/>
+    </row>
+    <row r="631">
+      <c r="B631" s="3"/>
+      <c r="C631" s="3"/>
+    </row>
+    <row r="632">
+      <c r="B632" s="3"/>
+      <c r="C632" s="3"/>
+    </row>
+    <row r="633">
+      <c r="B633" s="3"/>
+      <c r="C633" s="3"/>
+    </row>
+    <row r="634">
+      <c r="B634" s="3"/>
+      <c r="C634" s="3"/>
+    </row>
+    <row r="635">
+      <c r="B635" s="3"/>
+      <c r="C635" s="3"/>
+    </row>
+    <row r="636">
+      <c r="B636" s="3"/>
+      <c r="C636" s="3"/>
+    </row>
+    <row r="637">
+      <c r="B637" s="3"/>
+      <c r="C637" s="3"/>
+    </row>
+    <row r="638">
+      <c r="B638" s="3"/>
+      <c r="C638" s="3"/>
+    </row>
+    <row r="639">
+      <c r="B639" s="3"/>
+      <c r="C639" s="3"/>
+    </row>
+    <row r="640">
+      <c r="B640" s="3"/>
+      <c r="C640" s="3"/>
+    </row>
+    <row r="641">
+      <c r="B641" s="3"/>
+      <c r="C641" s="3"/>
+    </row>
+    <row r="642">
+      <c r="B642" s="3"/>
+      <c r="C642" s="3"/>
+    </row>
+    <row r="643">
+      <c r="B643" s="3"/>
+      <c r="C643" s="3"/>
+    </row>
+    <row r="644">
+      <c r="B644" s="3"/>
+      <c r="C644" s="3"/>
+    </row>
+    <row r="645">
+      <c r="B645" s="3"/>
+      <c r="C645" s="3"/>
+    </row>
+    <row r="646">
+      <c r="B646" s="3"/>
+      <c r="C646" s="3"/>
+    </row>
+    <row r="647">
+      <c r="B647" s="3"/>
+      <c r="C647" s="3"/>
+    </row>
+    <row r="648">
+      <c r="B648" s="3"/>
+      <c r="C648" s="3"/>
+    </row>
+    <row r="649">
+      <c r="B649" s="3"/>
+      <c r="C649" s="3"/>
+    </row>
+    <row r="650">
+      <c r="B650" s="3"/>
+      <c r="C650" s="3"/>
+    </row>
+    <row r="651">
+      <c r="B651" s="3"/>
+      <c r="C651" s="3"/>
+    </row>
+    <row r="652">
+      <c r="B652" s="3"/>
+      <c r="C652" s="3"/>
+    </row>
+    <row r="653">
+      <c r="B653" s="3"/>
+      <c r="C653" s="3"/>
+    </row>
+    <row r="654">
+      <c r="B654" s="3"/>
+      <c r="C654" s="3"/>
+    </row>
+    <row r="655">
+      <c r="B655" s="3"/>
+      <c r="C655" s="3"/>
+    </row>
+    <row r="656">
+      <c r="B656" s="3"/>
+      <c r="C656" s="3"/>
+    </row>
+    <row r="657">
+      <c r="B657" s="3"/>
+      <c r="C657" s="3"/>
+    </row>
+    <row r="658">
+      <c r="B658" s="3"/>
+      <c r="C658" s="3"/>
+    </row>
+    <row r="659">
+      <c r="B659" s="3"/>
+      <c r="C659" s="3"/>
+    </row>
+    <row r="660">
+      <c r="B660" s="3"/>
+      <c r="C660" s="3"/>
+    </row>
+    <row r="661">
+      <c r="B661" s="3"/>
+      <c r="C661" s="3"/>
+    </row>
+    <row r="662">
+      <c r="B662" s="3"/>
+      <c r="C662" s="3"/>
+    </row>
+    <row r="663">
+      <c r="B663" s="3"/>
+      <c r="C663" s="3"/>
+    </row>
+    <row r="664">
+      <c r="B664" s="3"/>
+      <c r="C664" s="3"/>
+    </row>
+    <row r="665">
+      <c r="B665" s="3"/>
+      <c r="C665" s="3"/>
+    </row>
+    <row r="666">
+      <c r="B666" s="3"/>
+      <c r="C666" s="3"/>
+    </row>
+    <row r="667">
+      <c r="B667" s="3"/>
+      <c r="C667" s="3"/>
+    </row>
+    <row r="668">
+      <c r="B668" s="3"/>
+      <c r="C668" s="3"/>
+    </row>
+    <row r="669">
+      <c r="B669" s="3"/>
+      <c r="C669" s="3"/>
+    </row>
+    <row r="670">
+      <c r="B670" s="3"/>
+      <c r="C670" s="3"/>
+    </row>
+    <row r="671">
+      <c r="B671" s="3"/>
+      <c r="C671" s="3"/>
+    </row>
+    <row r="672">
+      <c r="B672" s="3"/>
+      <c r="C672" s="3"/>
+    </row>
+    <row r="673">
+      <c r="B673" s="3"/>
+      <c r="C673" s="3"/>
+    </row>
+    <row r="674">
+      <c r="B674" s="3"/>
+      <c r="C674" s="3"/>
+    </row>
+    <row r="675">
+      <c r="B675" s="3"/>
+      <c r="C675" s="3"/>
+    </row>
+    <row r="676">
+      <c r="B676" s="3"/>
+      <c r="C676" s="3"/>
+    </row>
+    <row r="677">
+      <c r="B677" s="3"/>
+      <c r="C677" s="3"/>
+    </row>
+    <row r="678">
+      <c r="B678" s="3"/>
+      <c r="C678" s="3"/>
+    </row>
+    <row r="679">
+      <c r="B679" s="3"/>
+      <c r="C679" s="3"/>
+    </row>
+    <row r="680">
+      <c r="B680" s="3"/>
+      <c r="C680" s="3"/>
+    </row>
+    <row r="681">
+      <c r="B681" s="3"/>
+      <c r="C681" s="3"/>
+    </row>
+    <row r="682">
+      <c r="B682" s="3"/>
+      <c r="C682" s="3"/>
+    </row>
+    <row r="683">
+      <c r="B683" s="3"/>
+      <c r="C683" s="3"/>
+    </row>
+    <row r="684">
+      <c r="B684" s="3"/>
+      <c r="C684" s="3"/>
+    </row>
+    <row r="685">
+      <c r="B685" s="3"/>
+      <c r="C685" s="3"/>
+    </row>
+    <row r="686">
+      <c r="B686" s="3"/>
+      <c r="C686" s="3"/>
+    </row>
+    <row r="687">
+      <c r="B687" s="3"/>
+      <c r="C687" s="3"/>
+    </row>
+    <row r="688">
+      <c r="B688" s="3"/>
+      <c r="C688" s="3"/>
+    </row>
+    <row r="689">
+      <c r="B689" s="3"/>
+      <c r="C689" s="3"/>
+    </row>
+    <row r="690">
+      <c r="B690" s="3"/>
+      <c r="C690" s="3"/>
+    </row>
+    <row r="691">
+      <c r="B691" s="3"/>
+      <c r="C691" s="3"/>
+    </row>
+    <row r="692">
+      <c r="B692" s="3"/>
+      <c r="C692" s="3"/>
+    </row>
+    <row r="693">
+      <c r="B693" s="3"/>
+      <c r="C693" s="3"/>
+    </row>
+    <row r="694">
+      <c r="B694" s="3"/>
+      <c r="C694" s="3"/>
+    </row>
+    <row r="695">
+      <c r="B695" s="3"/>
+      <c r="C695" s="3"/>
+    </row>
+    <row r="696">
+      <c r="B696" s="3"/>
+      <c r="C696" s="3"/>
+    </row>
+    <row r="697">
+      <c r="B697" s="3"/>
+      <c r="C697" s="3"/>
+    </row>
+    <row r="698">
+      <c r="B698" s="3"/>
+      <c r="C698" s="3"/>
+    </row>
+    <row r="699">
+      <c r="B699" s="3"/>
+      <c r="C699" s="3"/>
+    </row>
+    <row r="700">
+      <c r="B700" s="3"/>
+      <c r="C700" s="3"/>
+    </row>
+    <row r="701">
+      <c r="B701" s="3"/>
+      <c r="C701" s="3"/>
+    </row>
+    <row r="702">
+      <c r="B702" s="3"/>
+      <c r="C702" s="3"/>
+    </row>
+    <row r="703">
+      <c r="B703" s="3"/>
+      <c r="C703" s="3"/>
+    </row>
+    <row r="704">
+      <c r="B704" s="3"/>
+      <c r="C704" s="3"/>
+    </row>
+    <row r="705">
+      <c r="B705" s="3"/>
+      <c r="C705" s="3"/>
+    </row>
+    <row r="706">
+      <c r="B706" s="3"/>
+      <c r="C706" s="3"/>
+    </row>
+    <row r="707">
+      <c r="B707" s="3"/>
+      <c r="C707" s="3"/>
+    </row>
+    <row r="708">
+      <c r="B708" s="3"/>
+      <c r="C708" s="3"/>
+    </row>
+    <row r="709">
+      <c r="B709" s="3"/>
+      <c r="C709" s="3"/>
+    </row>
+    <row r="710">
+      <c r="B710" s="3"/>
+      <c r="C710" s="3"/>
+    </row>
+    <row r="711">
+      <c r="B711" s="3"/>
+      <c r="C711" s="3"/>
+    </row>
+    <row r="712">
+      <c r="B712" s="3"/>
+      <c r="C712" s="3"/>
+    </row>
+    <row r="713">
+      <c r="B713" s="3"/>
+      <c r="C713" s="3"/>
+    </row>
+    <row r="714">
+      <c r="B714" s="3"/>
+      <c r="C714" s="3"/>
+    </row>
+    <row r="715">
+      <c r="B715" s="3"/>
+      <c r="C715" s="3"/>
+    </row>
+    <row r="716">
+      <c r="B716" s="3"/>
+      <c r="C716" s="3"/>
+    </row>
+    <row r="717">
+      <c r="B717" s="3"/>
+      <c r="C717" s="3"/>
+    </row>
+    <row r="718">
+      <c r="B718" s="3"/>
+      <c r="C718" s="3"/>
+    </row>
+    <row r="719">
+      <c r="B719" s="3"/>
+      <c r="C719" s="3"/>
+    </row>
+    <row r="720">
+      <c r="B720" s="3"/>
+      <c r="C720" s="3"/>
+    </row>
+    <row r="721">
+      <c r="B721" s="3"/>
+      <c r="C721" s="3"/>
+    </row>
+    <row r="722">
+      <c r="B722" s="3"/>
+      <c r="C722" s="3"/>
+    </row>
+    <row r="723">
+      <c r="B723" s="3"/>
+      <c r="C723" s="3"/>
+    </row>
+    <row r="724">
+      <c r="B724" s="3"/>
+      <c r="C724" s="3"/>
+    </row>
+    <row r="725">
+      <c r="B725" s="3"/>
+      <c r="C725" s="3"/>
+    </row>
+    <row r="726">
+      <c r="B726" s="3"/>
+      <c r="C726" s="3"/>
+    </row>
+    <row r="727">
+      <c r="B727" s="3"/>
+      <c r="C727" s="3"/>
+    </row>
+    <row r="728">
+      <c r="B728" s="3"/>
+      <c r="C728" s="3"/>
+    </row>
+    <row r="729">
+      <c r="B729" s="3"/>
+      <c r="C729" s="3"/>
+    </row>
+    <row r="730">
+      <c r="B730" s="3"/>
+      <c r="C730" s="3"/>
+    </row>
+    <row r="731">
+      <c r="B731" s="3"/>
+      <c r="C731" s="3"/>
+    </row>
+    <row r="732">
+      <c r="B732" s="3"/>
+      <c r="C732" s="3"/>
+    </row>
+    <row r="733">
+      <c r="B733" s="3"/>
+      <c r="C733" s="3"/>
+    </row>
+    <row r="734">
+      <c r="B734" s="3"/>
+      <c r="C734" s="3"/>
+    </row>
+    <row r="735">
+      <c r="B735" s="3"/>
+      <c r="C735" s="3"/>
+    </row>
+    <row r="736">
+      <c r="B736" s="3"/>
+      <c r="C736" s="3"/>
+    </row>
+    <row r="737">
+      <c r="B737" s="3"/>
+      <c r="C737" s="3"/>
+    </row>
+    <row r="738">
+      <c r="B738" s="3"/>
+      <c r="C738" s="3"/>
+    </row>
+    <row r="739">
+      <c r="B739" s="3"/>
+      <c r="C739" s="3"/>
+    </row>
+    <row r="740">
+      <c r="B740" s="3"/>
+      <c r="C740" s="3"/>
+    </row>
+    <row r="741">
+      <c r="B741" s="3"/>
+      <c r="C741" s="3"/>
+    </row>
+    <row r="742">
+      <c r="B742" s="3"/>
+      <c r="C742" s="3"/>
+    </row>
+    <row r="743">
+      <c r="B743" s="3"/>
+      <c r="C743" s="3"/>
+    </row>
+    <row r="744">
+      <c r="B744" s="3"/>
+      <c r="C744" s="3"/>
+    </row>
+    <row r="745">
+      <c r="B745" s="3"/>
+      <c r="C745" s="3"/>
+    </row>
+    <row r="746">
+      <c r="B746" s="3"/>
+      <c r="C746" s="3"/>
+    </row>
+    <row r="747">
+      <c r="B747" s="3"/>
+      <c r="C747" s="3"/>
+    </row>
+    <row r="748">
+      <c r="B748" s="3"/>
+      <c r="C748" s="3"/>
+    </row>
+    <row r="749">
+      <c r="B749" s="3"/>
+      <c r="C749" s="3"/>
+    </row>
+    <row r="750">
+      <c r="B750" s="3"/>
+      <c r="C750" s="3"/>
+    </row>
+    <row r="751">
+      <c r="B751" s="3"/>
+      <c r="C751" s="3"/>
+    </row>
+    <row r="752">
+      <c r="B752" s="3"/>
+      <c r="C752" s="3"/>
+    </row>
+    <row r="753">
+      <c r="B753" s="3"/>
+      <c r="C753" s="3"/>
+    </row>
+    <row r="754">
+      <c r="B754" s="3"/>
+      <c r="C754" s="3"/>
+    </row>
+    <row r="755">
+      <c r="B755" s="3"/>
+      <c r="C755" s="3"/>
+    </row>
+    <row r="756">
+      <c r="B756" s="3"/>
+      <c r="C756" s="3"/>
+    </row>
+    <row r="757">
+      <c r="B757" s="3"/>
+      <c r="C757" s="3"/>
+    </row>
+    <row r="758">
+      <c r="B758" s="3"/>
+      <c r="C758" s="3"/>
+    </row>
+    <row r="759">
+      <c r="B759" s="3"/>
+      <c r="C759" s="3"/>
+    </row>
+    <row r="760">
+      <c r="B760" s="3"/>
+      <c r="C760" s="3"/>
+    </row>
+    <row r="761">
+      <c r="B761" s="3"/>
+      <c r="C761" s="3"/>
+    </row>
+    <row r="762">
+      <c r="B762" s="3"/>
+      <c r="C762" s="3"/>
+    </row>
+    <row r="763">
+      <c r="B763" s="3"/>
+      <c r="C763" s="3"/>
+    </row>
+    <row r="764">
+      <c r="B764" s="3"/>
+      <c r="C764" s="3"/>
+    </row>
+    <row r="765">
+      <c r="B765" s="3"/>
+      <c r="C765" s="3"/>
+    </row>
+    <row r="766">
+      <c r="B766" s="3"/>
+      <c r="C766" s="3"/>
+    </row>
+    <row r="767">
+      <c r="B767" s="3"/>
+      <c r="C767" s="3"/>
+    </row>
+    <row r="768">
+      <c r="B768" s="3"/>
+      <c r="C768" s="3"/>
+    </row>
+    <row r="769">
+      <c r="B769" s="3"/>
+      <c r="C769" s="3"/>
+    </row>
+    <row r="770">
+      <c r="B770" s="3"/>
+      <c r="C770" s="3"/>
+    </row>
+    <row r="771">
+      <c r="B771" s="3"/>
+      <c r="C771" s="3"/>
+    </row>
+    <row r="772">
+      <c r="B772" s="3"/>
+      <c r="C772" s="3"/>
+    </row>
+    <row r="773">
+      <c r="B773" s="3"/>
+      <c r="C773" s="3"/>
+    </row>
+    <row r="774">
+      <c r="B774" s="3"/>
+      <c r="C774" s="3"/>
+    </row>
+    <row r="775">
+      <c r="B775" s="3"/>
+      <c r="C775" s="3"/>
+    </row>
+    <row r="776">
+      <c r="B776" s="3"/>
+      <c r="C776" s="3"/>
+    </row>
+    <row r="777">
+      <c r="B777" s="3"/>
+      <c r="C777" s="3"/>
+    </row>
+    <row r="778">
+      <c r="B778" s="3"/>
+      <c r="C778" s="3"/>
+    </row>
+    <row r="779">
+      <c r="B779" s="3"/>
+      <c r="C779" s="3"/>
+    </row>
+    <row r="780">
+      <c r="B780" s="3"/>
+      <c r="C780" s="3"/>
+    </row>
+    <row r="781">
+      <c r="B781" s="3"/>
+      <c r="C781" s="3"/>
+    </row>
+    <row r="782">
+      <c r="B782" s="3"/>
+      <c r="C782" s="3"/>
+    </row>
+    <row r="783">
+      <c r="B783" s="3"/>
+      <c r="C783" s="3"/>
+    </row>
+    <row r="784">
+      <c r="B784" s="3"/>
+      <c r="C784" s="3"/>
+    </row>
+    <row r="785">
+      <c r="B785" s="3"/>
+      <c r="C785" s="3"/>
+    </row>
+    <row r="786">
+      <c r="B786" s="3"/>
+      <c r="C786" s="3"/>
+    </row>
+    <row r="787">
+      <c r="B787" s="3"/>
+      <c r="C787" s="3"/>
+    </row>
+    <row r="788">
+      <c r="B788" s="3"/>
+      <c r="C788" s="3"/>
+    </row>
+    <row r="789">
+      <c r="B789" s="3"/>
+      <c r="C789" s="3"/>
+    </row>
+    <row r="790">
+      <c r="B790" s="3"/>
+      <c r="C790" s="3"/>
+    </row>
+    <row r="791">
+      <c r="B791" s="3"/>
+      <c r="C791" s="3"/>
+    </row>
+    <row r="792">
+      <c r="B792" s="3"/>
+      <c r="C792" s="3"/>
+    </row>
+    <row r="793">
+      <c r="B793" s="3"/>
+      <c r="C793" s="3"/>
+    </row>
+    <row r="794">
+      <c r="B794" s="3"/>
+      <c r="C794" s="3"/>
+    </row>
+    <row r="795">
+      <c r="B795" s="3"/>
+      <c r="C795" s="3"/>
+    </row>
+    <row r="796">
+      <c r="B796" s="3"/>
+      <c r="C796" s="3"/>
+    </row>
+    <row r="797">
+      <c r="B797" s="3"/>
+      <c r="C797" s="3"/>
+    </row>
+    <row r="798">
+      <c r="B798" s="3"/>
+      <c r="C798" s="3"/>
+    </row>
+    <row r="799">
+      <c r="B799" s="3"/>
+      <c r="C799" s="3"/>
+    </row>
+    <row r="800">
+      <c r="B800" s="3"/>
+      <c r="C800" s="3"/>
+    </row>
+    <row r="801">
+      <c r="B801" s="3"/>
+      <c r="C801" s="3"/>
+    </row>
+    <row r="802">
+      <c r="B802" s="3"/>
+      <c r="C802" s="3"/>
+    </row>
+    <row r="803">
+      <c r="B803" s="3"/>
+      <c r="C803" s="3"/>
+    </row>
+    <row r="804">
+      <c r="B804" s="3"/>
+      <c r="C804" s="3"/>
+    </row>
+    <row r="805">
+      <c r="B805" s="3"/>
+      <c r="C805" s="3"/>
+    </row>
+    <row r="806">
+      <c r="B806" s="3"/>
+      <c r="C806" s="3"/>
+    </row>
+    <row r="807">
+      <c r="B807" s="3"/>
+      <c r="C807" s="3"/>
+    </row>
+    <row r="808">
+      <c r="B808" s="3"/>
+      <c r="C808" s="3"/>
+    </row>
+    <row r="809">
+      <c r="B809" s="3"/>
+      <c r="C809" s="3"/>
+    </row>
+    <row r="810">
+      <c r="B810" s="3"/>
+      <c r="C810" s="3"/>
+    </row>
+    <row r="811">
+      <c r="B811" s="3"/>
+      <c r="C811" s="3"/>
+    </row>
+    <row r="812">
+      <c r="B812" s="3"/>
+      <c r="C812" s="3"/>
+    </row>
+    <row r="813">
+      <c r="B813" s="3"/>
+      <c r="C813" s="3"/>
+    </row>
+    <row r="814">
+      <c r="B814" s="3"/>
+      <c r="C814" s="3"/>
+    </row>
+    <row r="815">
+      <c r="B815" s="3"/>
+      <c r="C815" s="3"/>
+    </row>
+    <row r="816">
+      <c r="B816" s="3"/>
+      <c r="C816" s="3"/>
+    </row>
+    <row r="817">
+      <c r="B817" s="3"/>
+      <c r="C817" s="3"/>
+    </row>
+    <row r="818">
+      <c r="B818" s="3"/>
+      <c r="C818" s="3"/>
+    </row>
+    <row r="819">
+      <c r="B819" s="3"/>
+      <c r="C819" s="3"/>
+    </row>
+    <row r="820">
+      <c r="B820" s="3"/>
+      <c r="C820" s="3"/>
+    </row>
+    <row r="821">
+      <c r="B821" s="3"/>
+      <c r="C821" s="3"/>
+    </row>
+    <row r="822">
+      <c r="B822" s="3"/>
+      <c r="C822" s="3"/>
+    </row>
+    <row r="823">
+      <c r="B823" s="3"/>
+      <c r="C823" s="3"/>
+    </row>
+    <row r="824">
+      <c r="B824" s="3"/>
+      <c r="C824" s="3"/>
+    </row>
+    <row r="825">
+      <c r="B825" s="3"/>
+      <c r="C825" s="3"/>
+    </row>
+    <row r="826">
+      <c r="B826" s="3"/>
+      <c r="C826" s="3"/>
+    </row>
+    <row r="827">
+      <c r="B827" s="3"/>
+      <c r="C827" s="3"/>
+    </row>
+    <row r="828">
+      <c r="B828" s="3"/>
+      <c r="C828" s="3"/>
+    </row>
+    <row r="829">
+      <c r="B829" s="3"/>
+      <c r="C829" s="3"/>
+    </row>
+    <row r="830">
+      <c r="B830" s="3"/>
+      <c r="C830" s="3"/>
+    </row>
+    <row r="831">
+      <c r="B831" s="3"/>
+      <c r="C831" s="3"/>
+    </row>
+    <row r="832">
+      <c r="B832" s="3"/>
+      <c r="C832" s="3"/>
+    </row>
+    <row r="833">
+      <c r="B833" s="3"/>
+      <c r="C833" s="3"/>
+    </row>
+    <row r="834">
+      <c r="B834" s="3"/>
+      <c r="C834" s="3"/>
+    </row>
+    <row r="835">
+      <c r="B835" s="3"/>
+      <c r="C835" s="3"/>
+    </row>
+    <row r="836">
+      <c r="B836" s="3"/>
+      <c r="C836" s="3"/>
+    </row>
+    <row r="837">
+      <c r="B837" s="3"/>
+      <c r="C837" s="3"/>
+    </row>
+    <row r="838">
+      <c r="B838" s="3"/>
+      <c r="C838" s="3"/>
+    </row>
+    <row r="839">
+      <c r="B839" s="3"/>
+      <c r="C839" s="3"/>
+    </row>
+    <row r="840">
+      <c r="B840" s="3"/>
+      <c r="C840" s="3"/>
+    </row>
+    <row r="841">
+      <c r="B841" s="3"/>
+      <c r="C841" s="3"/>
+    </row>
+    <row r="842">
+      <c r="B842" s="3"/>
+      <c r="C842" s="3"/>
+    </row>
+    <row r="843">
+      <c r="B843" s="3"/>
+      <c r="C843" s="3"/>
+    </row>
+    <row r="844">
+      <c r="B844" s="3"/>
+      <c r="C844" s="3"/>
+    </row>
+    <row r="845">
+      <c r="B845" s="3"/>
+      <c r="C845" s="3"/>
+    </row>
+    <row r="846">
+      <c r="B846" s="3"/>
+      <c r="C846" s="3"/>
+    </row>
+    <row r="847">
+      <c r="B847" s="3"/>
+      <c r="C847" s="3"/>
+    </row>
+    <row r="848">
+      <c r="B848" s="3"/>
+      <c r="C848" s="3"/>
+    </row>
+    <row r="849">
+      <c r="B849" s="3"/>
+      <c r="C849" s="3"/>
+    </row>
+    <row r="850">
+      <c r="B850" s="3"/>
+      <c r="C850" s="3"/>
+    </row>
+    <row r="851">
+      <c r="B851" s="3"/>
+      <c r="C851" s="3"/>
+    </row>
+    <row r="852">
+      <c r="B852" s="3"/>
+      <c r="C852" s="3"/>
+    </row>
+    <row r="853">
+      <c r="B853" s="3"/>
+      <c r="C853" s="3"/>
+    </row>
+    <row r="854">
+      <c r="B854" s="3"/>
+      <c r="C854" s="3"/>
+    </row>
+    <row r="855">
+      <c r="B855" s="3"/>
+      <c r="C855" s="3"/>
+    </row>
+    <row r="856">
+      <c r="B856" s="3"/>
+      <c r="C856" s="3"/>
+    </row>
+    <row r="857">
+      <c r="B857" s="3"/>
+      <c r="C857" s="3"/>
+    </row>
+    <row r="858">
+      <c r="B858" s="3"/>
+      <c r="C858" s="3"/>
+    </row>
+    <row r="859">
+      <c r="B859" s="3"/>
+      <c r="C859" s="3"/>
+    </row>
+    <row r="860">
+      <c r="B860" s="3"/>
+      <c r="C860" s="3"/>
+    </row>
+    <row r="861">
+      <c r="B861" s="3"/>
+      <c r="C861" s="3"/>
+    </row>
+    <row r="862">
+      <c r="B862" s="3"/>
+      <c r="C862" s="3"/>
+    </row>
+    <row r="863">
+      <c r="B863" s="3"/>
+      <c r="C863" s="3"/>
+    </row>
+    <row r="864">
+      <c r="B864" s="3"/>
+      <c r="C864" s="3"/>
+    </row>
+    <row r="865">
+      <c r="B865" s="3"/>
+      <c r="C865" s="3"/>
+    </row>
+    <row r="866">
+      <c r="B866" s="3"/>
+      <c r="C866" s="3"/>
+    </row>
+    <row r="867">
+      <c r="B867" s="3"/>
+      <c r="C867" s="3"/>
+    </row>
+    <row r="868">
+      <c r="B868" s="3"/>
+      <c r="C868" s="3"/>
+    </row>
+    <row r="869">
+      <c r="B869" s="3"/>
+      <c r="C869" s="3"/>
+    </row>
+    <row r="870">
+      <c r="B870" s="3"/>
+      <c r="C870" s="3"/>
+    </row>
+    <row r="871">
+      <c r="B871" s="3"/>
+      <c r="C871" s="3"/>
+    </row>
+    <row r="872">
+      <c r="B872" s="3"/>
+      <c r="C872" s="3"/>
+    </row>
+    <row r="873">
+      <c r="B873" s="3"/>
+      <c r="C873" s="3"/>
+    </row>
+    <row r="874">
+      <c r="B874" s="3"/>
+      <c r="C874" s="3"/>
+    </row>
+    <row r="875">
+      <c r="B875" s="3"/>
+      <c r="C875" s="3"/>
+    </row>
+    <row r="876">
+      <c r="B876" s="3"/>
+      <c r="C876" s="3"/>
+    </row>
+    <row r="877">
+      <c r="B877" s="3"/>
+      <c r="C877" s="3"/>
+    </row>
+    <row r="878">
+      <c r="B878" s="3"/>
+      <c r="C878" s="3"/>
+    </row>
+    <row r="879">
+      <c r="B879" s="3"/>
+      <c r="C879" s="3"/>
+    </row>
+    <row r="880">
+      <c r="B880" s="3"/>
+      <c r="C880" s="3"/>
+    </row>
+    <row r="881">
+      <c r="B881" s="3"/>
+      <c r="C881" s="3"/>
+    </row>
+    <row r="882">
+      <c r="B882" s="3"/>
+      <c r="C882" s="3"/>
+    </row>
+    <row r="883">
+      <c r="B883" s="3"/>
+      <c r="C883" s="3"/>
+    </row>
+    <row r="884">
+      <c r="B884" s="3"/>
+      <c r="C884" s="3"/>
+    </row>
+    <row r="885">
+      <c r="B885" s="3"/>
+      <c r="C885" s="3"/>
+    </row>
+    <row r="886">
+      <c r="B886" s="3"/>
+      <c r="C886" s="3"/>
+    </row>
+    <row r="887">
+      <c r="B887" s="3"/>
+      <c r="C887" s="3"/>
+    </row>
+    <row r="888">
+      <c r="B888" s="3"/>
+      <c r="C888" s="3"/>
+    </row>
+    <row r="889">
+      <c r="B889" s="3"/>
+      <c r="C889" s="3"/>
+    </row>
+    <row r="890">
+      <c r="B890" s="3"/>
+      <c r="C890" s="3"/>
+    </row>
+    <row r="891">
+      <c r="B891" s="3"/>
+      <c r="C891" s="3"/>
+    </row>
+    <row r="892">
+      <c r="B892" s="3"/>
+      <c r="C892" s="3"/>
+    </row>
+    <row r="893">
+      <c r="B893" s="3"/>
+      <c r="C893" s="3"/>
+    </row>
+    <row r="894">
+      <c r="B894" s="3"/>
+      <c r="C894" s="3"/>
+    </row>
+    <row r="895">
+      <c r="B895" s="3"/>
+      <c r="C895" s="3"/>
+    </row>
+    <row r="896">
+      <c r="B896" s="3"/>
+      <c r="C896" s="3"/>
+    </row>
+    <row r="897">
+      <c r="B897" s="3"/>
+      <c r="C897" s="3"/>
+    </row>
+    <row r="898">
+      <c r="B898" s="3"/>
+      <c r="C898" s="3"/>
+    </row>
+    <row r="899">
+      <c r="B899" s="3"/>
+      <c r="C899" s="3"/>
+    </row>
+    <row r="900">
+      <c r="B900" s="3"/>
+      <c r="C900" s="3"/>
+    </row>
+    <row r="901">
+      <c r="B901" s="3"/>
+      <c r="C901" s="3"/>
+    </row>
+    <row r="902">
+      <c r="B902" s="3"/>
+      <c r="C902" s="3"/>
+    </row>
+    <row r="903">
+      <c r="B903" s="3"/>
+      <c r="C903" s="3"/>
+    </row>
+    <row r="904">
+      <c r="B904" s="3"/>
+      <c r="C904" s="3"/>
+    </row>
+    <row r="905">
+      <c r="B905" s="3"/>
+      <c r="C905" s="3"/>
+    </row>
+    <row r="906">
+      <c r="B906" s="3"/>
+      <c r="C906" s="3"/>
+    </row>
+    <row r="907">
+      <c r="B907" s="3"/>
+      <c r="C907" s="3"/>
+    </row>
+    <row r="908">
+      <c r="B908" s="3"/>
+      <c r="C908" s="3"/>
+    </row>
+    <row r="909">
+      <c r="B909" s="3"/>
+      <c r="C909" s="3"/>
+    </row>
+    <row r="910">
+      <c r="B910" s="3"/>
+      <c r="C910" s="3"/>
+    </row>
+    <row r="911">
+      <c r="B911" s="3"/>
+      <c r="C911" s="3"/>
+    </row>
+    <row r="912">
+      <c r="B912" s="3"/>
+      <c r="C912" s="3"/>
+    </row>
+    <row r="913">
+      <c r="B913" s="3"/>
+      <c r="C913" s="3"/>
+    </row>
+    <row r="914">
+      <c r="B914" s="3"/>
+      <c r="C914" s="3"/>
+    </row>
+    <row r="915">
+      <c r="B915" s="3"/>
+      <c r="C915" s="3"/>
+    </row>
+    <row r="916">
+      <c r="B916" s="3"/>
+      <c r="C916" s="3"/>
+    </row>
+    <row r="917">
+      <c r="B917" s="3"/>
+      <c r="C917" s="3"/>
+    </row>
+    <row r="918">
+      <c r="B918" s="3"/>
+      <c r="C918" s="3"/>
+    </row>
+    <row r="919">
+      <c r="B919" s="3"/>
+      <c r="C919" s="3"/>
+    </row>
+    <row r="920">
+      <c r="B920" s="3"/>
+      <c r="C920" s="3"/>
+    </row>
+    <row r="921">
+      <c r="B921" s="3"/>
+      <c r="C921" s="3"/>
+    </row>
+    <row r="922">
+      <c r="B922" s="3"/>
+      <c r="C922" s="3"/>
+    </row>
+    <row r="923">
+      <c r="B923" s="3"/>
+      <c r="C923" s="3"/>
+    </row>
+    <row r="924">
+      <c r="B924" s="3"/>
+      <c r="C924" s="3"/>
+    </row>
+    <row r="925">
+      <c r="B925" s="3"/>
+      <c r="C925" s="3"/>
+    </row>
+    <row r="926">
+      <c r="B926" s="3"/>
+      <c r="C926" s="3"/>
+    </row>
+    <row r="927">
+      <c r="B927" s="3"/>
+      <c r="C927" s="3"/>
+    </row>
+    <row r="928">
+      <c r="B928" s="3"/>
+      <c r="C928" s="3"/>
+    </row>
+    <row r="929">
+      <c r="B929" s="3"/>
+      <c r="C929" s="3"/>
+    </row>
+    <row r="930">
+      <c r="B930" s="3"/>
+      <c r="C930" s="3"/>
+    </row>
+    <row r="931">
+      <c r="B931" s="3"/>
+      <c r="C931" s="3"/>
+    </row>
+    <row r="932">
+      <c r="B932" s="3"/>
+      <c r="C932" s="3"/>
+    </row>
+    <row r="933">
+      <c r="B933" s="3"/>
+      <c r="C933" s="3"/>
+    </row>
+    <row r="934">
+      <c r="B934" s="3"/>
+      <c r="C934" s="3"/>
+    </row>
+    <row r="935">
+      <c r="B935" s="3"/>
+      <c r="C935" s="3"/>
+    </row>
+    <row r="936">
+      <c r="B936" s="3"/>
+      <c r="C936" s="3"/>
+    </row>
+    <row r="937">
+      <c r="B937" s="3"/>
+      <c r="C937" s="3"/>
+    </row>
+    <row r="938">
+      <c r="B938" s="3"/>
+      <c r="C938" s="3"/>
+    </row>
+    <row r="939">
+      <c r="B939" s="3"/>
+      <c r="C939" s="3"/>
+    </row>
+    <row r="940">
+      <c r="B940" s="3"/>
+      <c r="C940" s="3"/>
+    </row>
+    <row r="941">
+      <c r="B941" s="3"/>
+      <c r="C941" s="3"/>
+    </row>
+    <row r="942">
+      <c r="B942" s="3"/>
+      <c r="C942" s="3"/>
+    </row>
+    <row r="943">
+      <c r="B943" s="3"/>
+      <c r="C943" s="3"/>
+    </row>
+    <row r="944">
+      <c r="B944" s="3"/>
+      <c r="C944" s="3"/>
+    </row>
+    <row r="945">
+      <c r="B945" s="3"/>
+      <c r="C945" s="3"/>
+    </row>
+    <row r="946">
+      <c r="B946" s="3"/>
+      <c r="C946" s="3"/>
+    </row>
+    <row r="947">
+      <c r="B947" s="3"/>
+      <c r="C947" s="3"/>
+    </row>
+    <row r="948">
+      <c r="B948" s="3"/>
+      <c r="C948" s="3"/>
+    </row>
+    <row r="949">
+      <c r="B949" s="3"/>
+      <c r="C949" s="3"/>
+    </row>
+    <row r="950">
+      <c r="B950" s="3"/>
+      <c r="C950" s="3"/>
+    </row>
+    <row r="951">
+      <c r="B951" s="3"/>
+      <c r="C951" s="3"/>
+    </row>
+    <row r="952">
+      <c r="B952" s="3"/>
+      <c r="C952" s="3"/>
+    </row>
+    <row r="953">
+      <c r="B953" s="3"/>
+      <c r="C953" s="3"/>
+    </row>
+    <row r="954">
+      <c r="B954" s="3"/>
+      <c r="C954" s="3"/>
+    </row>
+    <row r="955">
+      <c r="B955" s="3"/>
+      <c r="C955" s="3"/>
+    </row>
+    <row r="956">
+      <c r="B956" s="3"/>
+      <c r="C956" s="3"/>
+    </row>
+    <row r="957">
+      <c r="B957" s="3"/>
+      <c r="C957" s="3"/>
+    </row>
+    <row r="958">
+      <c r="B958" s="3"/>
+      <c r="C958" s="3"/>
+    </row>
+    <row r="959">
+      <c r="B959" s="3"/>
+      <c r="C959" s="3"/>
+    </row>
+    <row r="960">
+      <c r="B960" s="3"/>
+      <c r="C960" s="3"/>
+    </row>
+    <row r="961">
+      <c r="B961" s="3"/>
+      <c r="C961" s="3"/>
+    </row>
+    <row r="962">
+      <c r="B962" s="3"/>
+      <c r="C962" s="3"/>
+    </row>
+    <row r="963">
+      <c r="B963" s="3"/>
+      <c r="C963" s="3"/>
+    </row>
+    <row r="964">
+      <c r="B964" s="3"/>
+      <c r="C964" s="3"/>
+    </row>
+    <row r="965">
+      <c r="B965" s="3"/>
+      <c r="C965" s="3"/>
+    </row>
+    <row r="966">
+      <c r="B966" s="3"/>
+      <c r="C966" s="3"/>
+    </row>
+    <row r="967">
+      <c r="B967" s="3"/>
+      <c r="C967" s="3"/>
+    </row>
+    <row r="968">
+      <c r="B968" s="3"/>
+      <c r="C968" s="3"/>
+    </row>
+    <row r="969">
+      <c r="B969" s="3"/>
+      <c r="C969" s="3"/>
+    </row>
+    <row r="970">
+      <c r="B970" s="3"/>
+      <c r="C970" s="3"/>
+    </row>
+    <row r="971">
+      <c r="B971" s="3"/>
+      <c r="C971" s="3"/>
+    </row>
+    <row r="972">
+      <c r="B972" s="3"/>
+      <c r="C972" s="3"/>
+    </row>
+    <row r="973">
+      <c r="B973" s="3"/>
+      <c r="C973" s="3"/>
+    </row>
+    <row r="974">
+      <c r="B974" s="3"/>
+      <c r="C974" s="3"/>
+    </row>
+    <row r="975">
+      <c r="B975" s="3"/>
+      <c r="C975" s="3"/>
+    </row>
+    <row r="976">
+      <c r="B976" s="3"/>
+      <c r="C976" s="3"/>
+    </row>
+    <row r="977">
+      <c r="B977" s="3"/>
+      <c r="C977" s="3"/>
+    </row>
+    <row r="978">
+      <c r="B978" s="3"/>
+      <c r="C978" s="3"/>
+    </row>
+    <row r="979">
+      <c r="B979" s="3"/>
+      <c r="C979" s="3"/>
+    </row>
+    <row r="980">
+      <c r="B980" s="3"/>
+      <c r="C980" s="3"/>
+    </row>
+    <row r="981">
+      <c r="B981" s="3"/>
+      <c r="C981" s="3"/>
+    </row>
+    <row r="982">
+      <c r="B982" s="3"/>
+      <c r="C982" s="3"/>
+    </row>
+    <row r="983">
+      <c r="B983" s="3"/>
+      <c r="C983" s="3"/>
+    </row>
+    <row r="984">
+      <c r="B984" s="3"/>
+      <c r="C984" s="3"/>
+    </row>
+    <row r="985">
+      <c r="B985" s="3"/>
+      <c r="C985" s="3"/>
+    </row>
+    <row r="986">
+      <c r="B986" s="3"/>
+      <c r="C986" s="3"/>
+    </row>
+    <row r="987">
+      <c r="B987" s="3"/>
+      <c r="C987" s="3"/>
+    </row>
+    <row r="988">
+      <c r="B988" s="3"/>
+      <c r="C988" s="3"/>
+    </row>
+    <row r="989">
+      <c r="B989" s="3"/>
+      <c r="C989" s="3"/>
+    </row>
+    <row r="990">
+      <c r="B990" s="3"/>
+      <c r="C990" s="3"/>
+    </row>
+    <row r="991">
+      <c r="B991" s="3"/>
+      <c r="C991" s="3"/>
+    </row>
+    <row r="992">
+      <c r="B992" s="3"/>
+      <c r="C992" s="3"/>
+    </row>
+    <row r="993">
+      <c r="B993" s="3"/>
+      <c r="C993" s="3"/>
+    </row>
+    <row r="994">
+      <c r="B994" s="3"/>
+      <c r="C994" s="3"/>
+    </row>
+    <row r="995">
+      <c r="B995" s="3"/>
+      <c r="C995" s="3"/>
+    </row>
+    <row r="996">
+      <c r="B996" s="3"/>
+      <c r="C996" s="3"/>
+    </row>
+    <row r="997">
+      <c r="B997" s="3"/>
+      <c r="C997" s="3"/>
+    </row>
+    <row r="998">
+      <c r="B998" s="3"/>
+      <c r="C998" s="3"/>
+    </row>
+    <row r="999">
+      <c r="B999" s="3"/>
+      <c r="C999" s="3"/>
+    </row>
+    <row r="1000">
+      <c r="B1000" s="3"/>
+      <c r="C1000" s="3"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>